<commit_message>
Error codes still do weird things like writing exclmamation makrs into the display dont know why
</commit_message>
<xml_diff>
--- a/DIC_doc.xlsx
+++ b/DIC_doc.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Technik\Technik 2020\04 - Electronics\13 - Software\DIC_Firmware_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606760B0-63C6-48C7-BED5-4FFCE800835E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A197AD1-4476-4E62-A5DF-8277D478717D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="75">
   <si>
     <t>C</t>
   </si>
@@ -236,6 +236,24 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -395,6 +413,14 @@
   <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -422,11 +448,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -457,11 +478,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -917,16 +935,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988E1A10-DA1E-4FA8-8A78-B3B11DC10728}">
   <dimension ref="A1:AP19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="AL3" sqref="AL3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="42" width="3.33203125" customWidth="1"/>
+    <col min="1" max="42" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -960,12 +978,12 @@
         <v>0</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="2">
-        <v>3</v>
-      </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="25"/>
+      <c r="R1" s="6">
+        <v>3</v>
+      </c>
+      <c r="S1" s="7"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="5"/>
       <c r="V1" s="1" t="s">
         <v>0</v>
       </c>
@@ -999,14 +1017,14 @@
         <v>0</v>
       </c>
       <c r="AL1" s="1"/>
-      <c r="AM1" s="2">
-        <v>3</v>
-      </c>
-      <c r="AN1" s="3"/>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="13"/>
-    </row>
-    <row r="2" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM1" s="6">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="8"/>
+      <c r="AP1" s="3"/>
+    </row>
+    <row r="2" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1046,10 +1064,10 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-      <c r="U2" s="25"/>
+      <c r="R2" s="9"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="11"/>
+      <c r="U2" s="5"/>
       <c r="V2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1089,12 +1107,12 @@
         <v>0</v>
       </c>
       <c r="AL2" s="1"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="6"/>
-      <c r="AO2" s="7"/>
-      <c r="AP2" s="13"/>
-    </row>
-    <row r="3" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM2" s="9"/>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="11"/>
+      <c r="AP2" s="3"/>
+    </row>
+    <row r="3" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1134,10 +1152,10 @@
         <v>10</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="25"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="5"/>
       <c r="V3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1154,35 +1172,37 @@
       </c>
       <c r="AB3" s="1"/>
       <c r="AC3" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AD3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AE3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="AF3" s="1"/>
-      <c r="AG3" s="1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="AE3" s="1"/>
+      <c r="AF3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="AH3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="AI3" s="1">
-        <v>5</v>
-      </c>
-      <c r="AJ3" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="AK3" s="1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="AL3" s="1"/>
-      <c r="AM3" s="5"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="7"/>
-      <c r="AP3" s="13"/>
-    </row>
-    <row r="4" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AM3" s="9"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="3"/>
+    </row>
+    <row r="4" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1214,31 +1234,31 @@
         <v>11</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="25"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="5"/>
       <c r="V4" s="1"/>
-      <c r="W4" s="24"/>
-      <c r="X4" s="24" t="s">
+      <c r="W4" s="4"/>
+      <c r="X4" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="Y4" s="24">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="24" t="s">
+      <c r="Y4" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AA4" s="24">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="24">
+      <c r="AA4" s="4">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="4">
         <v>4</v>
       </c>
-      <c r="AC4" s="24">
+      <c r="AC4" s="4">
         <v>2</v>
       </c>
-      <c r="AD4" s="24"/>
+      <c r="AD4" s="4"/>
       <c r="AE4" s="1"/>
       <c r="AF4" s="1">
         <v>1</v>
@@ -1257,971 +1277,971 @@
         <v>11</v>
       </c>
       <c r="AL4" s="1"/>
-      <c r="AM4" s="8"/>
-      <c r="AN4" s="9"/>
-      <c r="AO4" s="10"/>
-      <c r="AP4" s="13"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A5" s="25"/>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25"/>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="13"/>
-      <c r="W5" s="13"/>
-      <c r="X5" s="13"/>
-      <c r="Y5" s="13"/>
-      <c r="Z5" s="13"/>
-      <c r="AA5" s="13"/>
-      <c r="AB5" s="13"/>
-      <c r="AC5" s="13"/>
-      <c r="AD5" s="13"/>
-      <c r="AE5" s="13"/>
-      <c r="AF5" s="13"/>
-      <c r="AG5" s="13"/>
-      <c r="AH5" s="13"/>
-      <c r="AI5" s="13"/>
-      <c r="AJ5" s="13"/>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="13"/>
-      <c r="AM5" s="13"/>
-      <c r="AN5" s="13"/>
-      <c r="AO5" s="13"/>
-      <c r="AP5" s="13"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A6" s="24" t="s">
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="14"/>
+      <c r="AP4" s="3"/>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AG5" s="3"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="3"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="24">
-        <v>1</v>
-      </c>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24">
-        <v>1</v>
-      </c>
-      <c r="G6" s="24">
-        <v>0</v>
-      </c>
-      <c r="H6" s="24">
-        <v>0</v>
-      </c>
-      <c r="I6" s="24" t="s">
+      <c r="D6" s="4">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4">
+        <v>1</v>
+      </c>
+      <c r="G6" s="4">
+        <v>0</v>
+      </c>
+      <c r="H6" s="4">
+        <v>0</v>
+      </c>
+      <c r="I6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="24"/>
-      <c r="K6" s="24">
+      <c r="J6" s="4"/>
+      <c r="K6" s="4">
         <v>2</v>
       </c>
-      <c r="L6" s="24"/>
-      <c r="M6" s="24">
-        <v>1</v>
-      </c>
-      <c r="N6" s="24">
-        <v>0</v>
-      </c>
-      <c r="O6" s="24">
-        <v>0</v>
-      </c>
-      <c r="P6" s="24" t="s">
+      <c r="L6" s="4"/>
+      <c r="M6" s="4">
+        <v>1</v>
+      </c>
+      <c r="N6" s="4">
+        <v>0</v>
+      </c>
+      <c r="O6" s="4">
+        <v>0</v>
+      </c>
+      <c r="P6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="14">
-        <v>3</v>
-      </c>
-      <c r="S6" s="15"/>
-      <c r="T6" s="16"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="13"/>
-      <c r="W6" s="13"/>
-      <c r="X6" s="13"/>
-      <c r="Y6" s="13"/>
-      <c r="Z6" s="13"/>
-      <c r="AA6" s="13"/>
-      <c r="AB6" s="13"/>
-      <c r="AC6" s="13"/>
-      <c r="AD6" s="13"/>
-      <c r="AE6" s="13"/>
-      <c r="AF6" s="13"/>
-      <c r="AG6" s="13"/>
-      <c r="AH6" s="13"/>
-      <c r="AI6" s="13"/>
-      <c r="AJ6" s="13"/>
-      <c r="AK6" s="13"/>
-      <c r="AL6" s="13"/>
-      <c r="AM6" s="13"/>
-      <c r="AN6" s="13"/>
-      <c r="AO6" s="13"/>
-      <c r="AP6" s="13"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A7" s="24" t="s">
+      <c r="Q6" s="4"/>
+      <c r="R6" s="15">
+        <v>3</v>
+      </c>
+      <c r="S6" s="16"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="5"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
+      <c r="AA6" s="3"/>
+      <c r="AB6" s="3"/>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="24">
-        <v>1</v>
-      </c>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24">
-        <v>1</v>
-      </c>
-      <c r="G7" s="24">
-        <v>0</v>
-      </c>
-      <c r="H7" s="24">
-        <v>0</v>
-      </c>
-      <c r="I7" s="24" t="s">
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4">
+        <v>0</v>
+      </c>
+      <c r="H7" s="4">
+        <v>0</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="24"/>
-      <c r="K7" s="24">
+      <c r="J7" s="4"/>
+      <c r="K7" s="4">
         <v>2</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="24">
-        <v>1</v>
-      </c>
-      <c r="N7" s="24">
-        <v>0</v>
-      </c>
-      <c r="O7" s="24">
-        <v>0</v>
-      </c>
-      <c r="P7" s="24" t="s">
+      <c r="L7" s="4"/>
+      <c r="M7" s="4">
+        <v>1</v>
+      </c>
+      <c r="N7" s="4">
+        <v>0</v>
+      </c>
+      <c r="O7" s="4">
+        <v>0</v>
+      </c>
+      <c r="P7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="Q7" s="24"/>
-      <c r="R7" s="17"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="19"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="13"/>
-      <c r="W7" s="13"/>
-      <c r="X7" s="13"/>
-      <c r="Y7" s="13"/>
-      <c r="Z7" s="13"/>
-      <c r="AA7" s="13"/>
-      <c r="AB7" s="13"/>
-      <c r="AC7" s="13"/>
-      <c r="AD7" s="13"/>
-      <c r="AE7" s="13"/>
-      <c r="AF7" s="13"/>
-      <c r="AG7" s="13"/>
-      <c r="AH7" s="13"/>
-      <c r="AI7" s="13"/>
-      <c r="AJ7" s="13"/>
-      <c r="AK7" s="13"/>
-      <c r="AL7" s="13"/>
-      <c r="AM7" s="13"/>
-      <c r="AN7" s="13"/>
-      <c r="AO7" s="13"/>
-      <c r="AP7" s="13"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A8" s="24" t="s">
+      <c r="Q7" s="4"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="19"/>
+      <c r="T7" s="20"/>
+      <c r="U7" s="5"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
+      <c r="AA7" s="3"/>
+      <c r="AB7" s="3"/>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AG7" s="3"/>
+      <c r="AH7" s="3"/>
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+      <c r="AK7" s="3"/>
+      <c r="AL7" s="3"/>
+      <c r="AM7" s="3"/>
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AP7" s="3"/>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24">
-        <v>1</v>
-      </c>
-      <c r="G8" s="24">
-        <v>0</v>
-      </c>
-      <c r="H8" s="24">
-        <v>0</v>
-      </c>
-      <c r="I8" s="24" t="s">
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="G8" s="4">
+        <v>0</v>
+      </c>
+      <c r="H8" s="4">
+        <v>0</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="24"/>
-      <c r="K8" s="24"/>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24"/>
-      <c r="N8" s="24"/>
-      <c r="O8" s="24"/>
-      <c r="P8" s="24"/>
-      <c r="Q8" s="24"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="18"/>
-      <c r="T8" s="19"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="13"/>
-      <c r="W8" s="13"/>
-      <c r="X8" s="13"/>
-      <c r="Y8" s="13"/>
-      <c r="Z8" s="13"/>
-      <c r="AA8" s="13"/>
-      <c r="AB8" s="13"/>
-      <c r="AC8" s="13"/>
-      <c r="AD8" s="13"/>
-      <c r="AE8" s="13"/>
-      <c r="AF8" s="13"/>
-      <c r="AG8" s="13"/>
-      <c r="AH8" s="13"/>
-      <c r="AI8" s="13"/>
-      <c r="AJ8" s="13"/>
-      <c r="AK8" s="13"/>
-      <c r="AL8" s="13"/>
-      <c r="AM8" s="13"/>
-      <c r="AN8" s="13"/>
-      <c r="AO8" s="13"/>
-      <c r="AP8" s="13"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A9" s="24" t="s">
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
+      <c r="M8" s="4"/>
+      <c r="N8" s="4"/>
+      <c r="O8" s="4"/>
+      <c r="P8" s="4"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="19"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="5"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
+      <c r="AA8" s="3"/>
+      <c r="AB8" s="3"/>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AG8" s="3"/>
+      <c r="AH8" s="3"/>
+      <c r="AI8" s="3"/>
+      <c r="AJ8" s="3"/>
+      <c r="AK8" s="3"/>
+      <c r="AL8" s="3"/>
+      <c r="AM8" s="3"/>
+      <c r="AN8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AP8" s="3"/>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24">
-        <v>9</v>
-      </c>
-      <c r="F9" s="24">
-        <v>0</v>
-      </c>
-      <c r="G9" s="24" t="s">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4">
+        <v>9</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24" t="s">
+      <c r="H9" s="4"/>
+      <c r="I9" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24">
-        <v>9</v>
-      </c>
-      <c r="L9" s="24">
-        <v>0</v>
-      </c>
-      <c r="M9" s="24" t="s">
+      <c r="J9" s="4"/>
+      <c r="K9" s="4">
+        <v>9</v>
+      </c>
+      <c r="L9" s="4">
+        <v>0</v>
+      </c>
+      <c r="M9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="21"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
-      <c r="Y9" s="13"/>
-      <c r="Z9" s="13"/>
-      <c r="AA9" s="13"/>
-      <c r="AB9" s="13"/>
-      <c r="AC9" s="13"/>
-      <c r="AD9" s="13"/>
-      <c r="AE9" s="13"/>
-      <c r="AF9" s="13"/>
-      <c r="AG9" s="13"/>
-      <c r="AH9" s="13"/>
-      <c r="AI9" s="13"/>
-      <c r="AJ9" s="13"/>
-      <c r="AK9" s="13"/>
-      <c r="AL9" s="13"/>
-      <c r="AM9" s="13"/>
-      <c r="AN9" s="13"/>
-      <c r="AO9" s="13"/>
-      <c r="AP9" s="13"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="O10" s="25"/>
-      <c r="P10" s="25"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
-      <c r="Y10" s="13"/>
-      <c r="Z10" s="13"/>
-      <c r="AA10" s="13"/>
-      <c r="AB10" s="13"/>
-      <c r="AC10" s="13"/>
-      <c r="AD10" s="13"/>
-      <c r="AE10" s="13"/>
-      <c r="AF10" s="13"/>
-      <c r="AG10" s="13"/>
-      <c r="AH10" s="13"/>
-      <c r="AI10" s="13"/>
-      <c r="AJ10" s="13"/>
-      <c r="AK10" s="13"/>
-      <c r="AL10" s="13"/>
-      <c r="AM10" s="13"/>
-      <c r="AN10" s="13"/>
-      <c r="AO10" s="13"/>
-      <c r="AP10" s="13"/>
-    </row>
-    <row r="11" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="24" t="s">
+      <c r="N9" s="4"/>
+      <c r="O9" s="4"/>
+      <c r="P9" s="4"/>
+      <c r="Q9" s="4"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="22"/>
+      <c r="T9" s="23"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
+      <c r="AA9" s="3"/>
+      <c r="AB9" s="3"/>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
+      <c r="AG9" s="3"/>
+      <c r="AH9" s="3"/>
+      <c r="AI9" s="3"/>
+      <c r="AJ9" s="3"/>
+      <c r="AK9" s="3"/>
+      <c r="AL9" s="3"/>
+      <c r="AM9" s="3"/>
+      <c r="AN9" s="3"/>
+      <c r="AO9" s="3"/>
+      <c r="AP9" s="3"/>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5"/>
+      <c r="Q10" s="5"/>
+      <c r="R10" s="5"/>
+      <c r="S10" s="5"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
+      <c r="AA10" s="3"/>
+      <c r="AB10" s="3"/>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
+      <c r="AG10" s="3"/>
+      <c r="AH10" s="3"/>
+      <c r="AI10" s="3"/>
+      <c r="AJ10" s="3"/>
+      <c r="AK10" s="3"/>
+      <c r="AL10" s="3"/>
+      <c r="AM10" s="3"/>
+      <c r="AN10" s="3"/>
+      <c r="AO10" s="3"/>
+      <c r="AP10" s="3"/>
+    </row>
+    <row r="11" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24">
-        <v>9</v>
-      </c>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24" t="s">
+      <c r="B11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4">
+        <v>9</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24">
-        <v>1</v>
-      </c>
-      <c r="L11" s="24">
-        <v>1</v>
-      </c>
-      <c r="M11" s="24">
+      <c r="I11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="4">
+        <v>1</v>
+      </c>
+      <c r="L11" s="4">
+        <v>1</v>
+      </c>
+      <c r="M11" s="4">
         <v>2</v>
       </c>
-      <c r="N11" s="24" t="s">
+      <c r="N11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O11" s="24" t="s">
+      <c r="O11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" s="24"/>
-      <c r="R11" s="14">
-        <v>3</v>
-      </c>
-      <c r="S11" s="15"/>
-      <c r="T11" s="16"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="24" t="s">
+      <c r="Q11" s="4"/>
+      <c r="R11" s="15">
+        <v>3</v>
+      </c>
+      <c r="S11" s="16"/>
+      <c r="T11" s="17"/>
+      <c r="U11" s="5"/>
+      <c r="V11" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="W11" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="X11" s="24"/>
-      <c r="Y11" s="24">
-        <v>9</v>
-      </c>
-      <c r="Z11" s="24"/>
-      <c r="AA11" s="24"/>
-      <c r="AB11" s="24" t="s">
+      <c r="W11" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="X11" s="4"/>
+      <c r="Y11" s="4">
+        <v>9</v>
+      </c>
+      <c r="Z11" s="4"/>
+      <c r="AA11" s="4"/>
+      <c r="AB11" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AC11" s="24" t="s">
+      <c r="AC11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AD11" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE11" s="24"/>
-      <c r="AF11" s="24">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="24">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="24">
+      <c r="AD11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="4"/>
+      <c r="AF11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="4">
         <v>2</v>
       </c>
-      <c r="AI11" s="24" t="s">
+      <c r="AI11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AJ11" s="24" t="s">
+      <c r="AJ11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AK11" s="24" t="s">
+      <c r="AK11" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="AL11" s="24"/>
-      <c r="AM11" s="14">
-        <v>3</v>
-      </c>
-      <c r="AN11" s="15"/>
-      <c r="AO11" s="16"/>
-      <c r="AP11" s="13"/>
-    </row>
-    <row r="12" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="24" t="s">
+      <c r="AL11" s="4"/>
+      <c r="AM11" s="15">
+        <v>3</v>
+      </c>
+      <c r="AN11" s="16"/>
+      <c r="AO11" s="17"/>
+      <c r="AP11" s="3"/>
+    </row>
+    <row r="12" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="24" t="s">
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24">
-        <v>1</v>
-      </c>
-      <c r="F12" s="24" t="s">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="24">
-        <v>1</v>
-      </c>
-      <c r="H12" s="24">
-        <v>3</v>
-      </c>
-      <c r="I12" s="24" t="s">
+      <c r="G12" s="4">
+        <v>1</v>
+      </c>
+      <c r="H12" s="4">
+        <v>3</v>
+      </c>
+      <c r="I12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="24">
+      <c r="J12" s="4">
         <v>4</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="4">
         <v>5</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="4">
         <v>6</v>
       </c>
-      <c r="M12" s="24"/>
-      <c r="N12" s="24"/>
-      <c r="O12" s="24"/>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="24"/>
-      <c r="R12" s="17"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="19"/>
-      <c r="U12" s="25"/>
-      <c r="V12" s="24" t="s">
+      <c r="M12" s="4"/>
+      <c r="N12" s="4"/>
+      <c r="O12" s="4"/>
+      <c r="P12" s="4"/>
+      <c r="Q12" s="4"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="19"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="5"/>
+      <c r="V12" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="W12" s="24" t="s">
+      <c r="W12" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="X12" s="24" t="s">
+      <c r="X12" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="24" t="s">
+      <c r="Y12" s="4"/>
+      <c r="Z12" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB12" s="24">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="24">
-        <v>3</v>
-      </c>
-      <c r="AD12" s="24" t="s">
+      <c r="AB12" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="4">
+        <v>3</v>
+      </c>
+      <c r="AD12" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AE12" s="24">
+      <c r="AE12" s="4">
         <v>4</v>
       </c>
-      <c r="AF12" s="24">
+      <c r="AF12" s="4">
         <v>5</v>
       </c>
-      <c r="AG12" s="24">
+      <c r="AG12" s="4">
         <v>6</v>
       </c>
-      <c r="AH12" s="24"/>
-      <c r="AI12" s="24"/>
-      <c r="AJ12" s="24"/>
-      <c r="AK12" s="24"/>
-      <c r="AL12" s="24"/>
-      <c r="AM12" s="17"/>
-      <c r="AN12" s="18"/>
-      <c r="AO12" s="19"/>
-      <c r="AP12" s="13"/>
-    </row>
-    <row r="13" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="24" t="s">
+      <c r="AH12" s="4"/>
+      <c r="AI12" s="4"/>
+      <c r="AJ12" s="4"/>
+      <c r="AK12" s="4"/>
+      <c r="AL12" s="4"/>
+      <c r="AM12" s="18"/>
+      <c r="AN12" s="19"/>
+      <c r="AO12" s="20"/>
+      <c r="AP12" s="3"/>
+    </row>
+    <row r="13" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="24"/>
-      <c r="E13" s="24">
-        <v>1</v>
-      </c>
-      <c r="F13" s="24" t="s">
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="24">
-        <v>1</v>
-      </c>
-      <c r="H13" s="24">
+      <c r="G13" s="4">
+        <v>1</v>
+      </c>
+      <c r="H13" s="4">
         <v>4</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="24">
+      <c r="J13" s="4">
         <v>6</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="4">
         <v>7</v>
       </c>
-      <c r="L13" s="24">
+      <c r="L13" s="4">
         <v>8</v>
       </c>
-      <c r="M13" s="24"/>
-      <c r="N13" s="24"/>
-      <c r="O13" s="24"/>
-      <c r="P13" s="24"/>
-      <c r="Q13" s="24"/>
-      <c r="R13" s="17"/>
-      <c r="S13" s="18"/>
-      <c r="T13" s="19"/>
-      <c r="U13" s="25"/>
-      <c r="V13" s="24" t="s">
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
+      <c r="O13" s="4"/>
+      <c r="P13" s="4"/>
+      <c r="Q13" s="4"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="19"/>
+      <c r="T13" s="20"/>
+      <c r="U13" s="5"/>
+      <c r="V13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="W13" s="24" t="s">
+      <c r="W13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="X13" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="24" t="s">
+      <c r="X13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="4"/>
+      <c r="Z13" s="4">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AB13" s="24">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="24">
+      <c r="AB13" s="4">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="4">
         <v>4</v>
       </c>
-      <c r="AD13" s="24" t="s">
+      <c r="AD13" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AE13" s="24">
+      <c r="AE13" s="4">
         <v>6</v>
       </c>
-      <c r="AF13" s="24">
+      <c r="AF13" s="4">
         <v>7</v>
       </c>
-      <c r="AG13" s="24">
+      <c r="AG13" s="4">
         <v>8</v>
       </c>
-      <c r="AH13" s="24"/>
-      <c r="AI13" s="24"/>
-      <c r="AJ13" s="24"/>
-      <c r="AK13" s="24"/>
-      <c r="AL13" s="24"/>
-      <c r="AM13" s="17"/>
-      <c r="AN13" s="18"/>
-      <c r="AO13" s="19"/>
-      <c r="AP13" s="13"/>
-    </row>
-    <row r="14" spans="1:42" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="24" t="s">
+      <c r="AH13" s="4"/>
+      <c r="AI13" s="4"/>
+      <c r="AJ13" s="4"/>
+      <c r="AK13" s="4"/>
+      <c r="AL13" s="4"/>
+      <c r="AM13" s="18"/>
+      <c r="AN13" s="19"/>
+      <c r="AO13" s="20"/>
+      <c r="AP13" s="3"/>
+    </row>
+    <row r="14" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24">
-        <v>3</v>
-      </c>
-      <c r="E14" s="24">
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
+        <v>3</v>
+      </c>
+      <c r="E14" s="4">
         <v>4</v>
       </c>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="24" t="s">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="24"/>
-      <c r="K14" s="24">
-        <v>1</v>
-      </c>
-      <c r="L14" s="24">
-        <v>3</v>
-      </c>
-      <c r="M14" s="24">
-        <v>9</v>
-      </c>
-      <c r="N14" s="24" t="s">
+      <c r="I14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="4"/>
+      <c r="K14" s="4">
+        <v>1</v>
+      </c>
+      <c r="L14" s="4">
+        <v>3</v>
+      </c>
+      <c r="M14" s="4">
+        <v>9</v>
+      </c>
+      <c r="N14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="24" t="s">
+      <c r="O14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="P14" s="24"/>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="20"/>
-      <c r="S14" s="21"/>
-      <c r="T14" s="22"/>
-      <c r="U14" s="25"/>
-      <c r="V14" s="24" t="s">
+      <c r="P14" s="4"/>
+      <c r="Q14" s="4"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="22"/>
+      <c r="T14" s="23"/>
+      <c r="U14" s="5"/>
+      <c r="V14" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="W14" s="24" t="s">
+      <c r="W14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24">
-        <v>3</v>
-      </c>
-      <c r="Z14" s="24">
+      <c r="X14" s="4"/>
+      <c r="Y14" s="4">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="4">
         <v>4</v>
       </c>
-      <c r="AA14" s="24"/>
-      <c r="AB14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="24" t="s">
+      <c r="AA14" s="4"/>
+      <c r="AB14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AD14" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE14" s="24"/>
-      <c r="AF14" s="24">
-        <v>1</v>
-      </c>
-      <c r="AG14" s="24">
-        <v>3</v>
-      </c>
-      <c r="AH14" s="24">
-        <v>9</v>
-      </c>
-      <c r="AI14" s="24" t="s">
+      <c r="AD14" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="4"/>
+      <c r="AF14" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="4">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="4">
+        <v>9</v>
+      </c>
+      <c r="AI14" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="AJ14" s="24" t="s">
+      <c r="AJ14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="AK14" s="24"/>
-      <c r="AL14" s="24"/>
-      <c r="AM14" s="20"/>
-      <c r="AN14" s="21"/>
-      <c r="AO14" s="22"/>
-      <c r="AP14" s="13"/>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="25"/>
-      <c r="R15" s="25"/>
-      <c r="S15" s="25"/>
-      <c r="T15" s="25"/>
-      <c r="U15" s="25"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
-      <c r="Y15" s="13"/>
-      <c r="Z15" s="13"/>
-      <c r="AA15" s="13"/>
-      <c r="AB15" s="13"/>
-      <c r="AC15" s="13"/>
-      <c r="AD15" s="13"/>
-      <c r="AE15" s="13"/>
-      <c r="AF15" s="13"/>
-      <c r="AG15" s="13"/>
-      <c r="AH15" s="13"/>
-      <c r="AI15" s="13"/>
-      <c r="AJ15" s="13"/>
-      <c r="AK15" s="13"/>
-      <c r="AL15" s="13"/>
-      <c r="AM15" s="13"/>
-      <c r="AN15" s="13"/>
-      <c r="AO15" s="13"/>
-      <c r="AP15" s="13"/>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A16" s="24"/>
-      <c r="B16" s="24"/>
-      <c r="C16" s="23">
-        <v>1</v>
-      </c>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23">
-        <v>0</v>
-      </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23">
+      <c r="AK14" s="4"/>
+      <c r="AL14" s="4"/>
+      <c r="AM14" s="21"/>
+      <c r="AN14" s="22"/>
+      <c r="AO14" s="23"/>
+      <c r="AP14" s="3"/>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
+      <c r="V15" s="3"/>
+      <c r="W15" s="3"/>
+      <c r="X15" s="3"/>
+      <c r="Y15" s="3"/>
+      <c r="Z15" s="3"/>
+      <c r="AA15" s="3"/>
+      <c r="AB15" s="3"/>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
+      <c r="AG15" s="3"/>
+      <c r="AH15" s="3"/>
+      <c r="AI15" s="3"/>
+      <c r="AJ15" s="3"/>
+      <c r="AK15" s="3"/>
+      <c r="AL15" s="3"/>
+      <c r="AM15" s="3"/>
+      <c r="AN15" s="3"/>
+      <c r="AO15" s="3"/>
+      <c r="AP15" s="3"/>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="24">
+        <v>1</v>
+      </c>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24">
+        <v>0</v>
+      </c>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24">
         <v>5</v>
       </c>
-      <c r="J16" s="23"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="23">
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24">
         <v>5</v>
       </c>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23">
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+      <c r="O16" s="24">
         <v>4</v>
       </c>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
-      <c r="T16" s="24"/>
-      <c r="U16" s="25"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
-      <c r="Y16" s="13"/>
-      <c r="Z16" s="13"/>
-      <c r="AA16" s="13"/>
-      <c r="AB16" s="13"/>
-      <c r="AC16" s="13"/>
-      <c r="AD16" s="13"/>
-      <c r="AE16" s="13"/>
-      <c r="AF16" s="13"/>
-      <c r="AG16" s="13"/>
-      <c r="AH16" s="13"/>
-      <c r="AI16" s="13"/>
-      <c r="AJ16" s="13"/>
-      <c r="AK16" s="13"/>
-      <c r="AL16" s="13"/>
-      <c r="AM16" s="13"/>
-      <c r="AN16" s="13"/>
-      <c r="AO16" s="13"/>
-      <c r="AP16" s="13"/>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
-      <c r="T17" s="24"/>
-      <c r="U17" s="25"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
-      <c r="Y17" s="13"/>
-      <c r="Z17" s="13"/>
-      <c r="AA17" s="13"/>
-      <c r="AB17" s="13"/>
-      <c r="AC17" s="13"/>
-      <c r="AD17" s="13"/>
-      <c r="AE17" s="13"/>
-      <c r="AF17" s="13"/>
-      <c r="AG17" s="13"/>
-      <c r="AH17" s="13"/>
-      <c r="AI17" s="13"/>
-      <c r="AJ17" s="13"/>
-      <c r="AK17" s="13"/>
-      <c r="AL17" s="13"/>
-      <c r="AM17" s="13"/>
-      <c r="AN17" s="13"/>
-      <c r="AO17" s="13"/>
-      <c r="AP17" s="13"/>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A18" s="24"/>
-      <c r="B18" s="24"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="23"/>
-      <c r="M18" s="23"/>
-      <c r="N18" s="23"/>
-      <c r="O18" s="23"/>
-      <c r="P18" s="23"/>
-      <c r="Q18" s="23"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
-      <c r="T18" s="24"/>
-      <c r="U18" s="25"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
-      <c r="Y18" s="13"/>
-      <c r="Z18" s="13"/>
-      <c r="AA18" s="13"/>
-      <c r="AB18" s="13"/>
-      <c r="AC18" s="13"/>
-      <c r="AD18" s="13"/>
-      <c r="AE18" s="13"/>
-      <c r="AF18" s="13"/>
-      <c r="AG18" s="13"/>
-      <c r="AH18" s="13"/>
-      <c r="AI18" s="13"/>
-      <c r="AJ18" s="13"/>
-      <c r="AK18" s="13"/>
-      <c r="AL18" s="13"/>
-      <c r="AM18" s="13"/>
-      <c r="AN18" s="13"/>
-      <c r="AO18" s="13"/>
-      <c r="AP18" s="13"/>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.3">
-      <c r="A19" s="24"/>
-      <c r="B19" s="24"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-      <c r="N19" s="23"/>
-      <c r="O19" s="23"/>
-      <c r="P19" s="23"/>
-      <c r="Q19" s="23"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
-      <c r="T19" s="24"/>
-      <c r="U19" s="25"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
-      <c r="Y19" s="13"/>
-      <c r="Z19" s="13"/>
-      <c r="AA19" s="13"/>
-      <c r="AB19" s="13"/>
-      <c r="AC19" s="13"/>
-      <c r="AD19" s="13"/>
-      <c r="AE19" s="13"/>
-      <c r="AF19" s="13"/>
-      <c r="AG19" s="13"/>
-      <c r="AH19" s="13"/>
-      <c r="AI19" s="13"/>
-      <c r="AJ19" s="13"/>
-      <c r="AK19" s="13"/>
-      <c r="AL19" s="13"/>
-      <c r="AM19" s="13"/>
-      <c r="AN19" s="13"/>
-      <c r="AO19" s="13"/>
-      <c r="AP19" s="13"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="3"/>
+      <c r="W16" s="3"/>
+      <c r="X16" s="3"/>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3"/>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3"/>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3"/>
+      <c r="AK16" s="3"/>
+      <c r="AL16" s="3"/>
+      <c r="AM16" s="3"/>
+      <c r="AN16" s="3"/>
+      <c r="AO16" s="3"/>
+      <c r="AP16" s="3"/>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
+      <c r="K17" s="24"/>
+      <c r="L17" s="24"/>
+      <c r="M17" s="24"/>
+      <c r="N17" s="24"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="4"/>
+      <c r="S17" s="4"/>
+      <c r="T17" s="4"/>
+      <c r="U17" s="5"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3"/>
+      <c r="AN17" s="3"/>
+      <c r="AO17" s="3"/>
+      <c r="AP17" s="3"/>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
+      <c r="M18" s="24"/>
+      <c r="N18" s="24"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="4"/>
+      <c r="S18" s="4"/>
+      <c r="T18" s="4"/>
+      <c r="U18" s="5"/>
+      <c r="V18" s="3"/>
+      <c r="W18" s="3"/>
+      <c r="X18" s="3"/>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3"/>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3"/>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3"/>
+      <c r="AK18" s="3"/>
+      <c r="AL18" s="3"/>
+      <c r="AM18" s="3"/>
+      <c r="AN18" s="3"/>
+      <c r="AO18" s="3"/>
+      <c r="AP18" s="3"/>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="24"/>
+      <c r="M19" s="24"/>
+      <c r="N19" s="24"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="4"/>
+      <c r="S19" s="4"/>
+      <c r="T19" s="4"/>
+      <c r="U19" s="5"/>
+      <c r="V19" s="3"/>
+      <c r="W19" s="3"/>
+      <c r="X19" s="3"/>
+      <c r="Y19" s="3"/>
+      <c r="Z19" s="3"/>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="3"/>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
+      <c r="AG19" s="3"/>
+      <c r="AH19" s="3"/>
+      <c r="AI19" s="3"/>
+      <c r="AJ19" s="3"/>
+      <c r="AK19" s="3"/>
+      <c r="AL19" s="3"/>
+      <c r="AM19" s="3"/>
+      <c r="AN19" s="3"/>
+      <c r="AO19" s="3"/>
+      <c r="AP19" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C16:E19"/>
+    <mergeCell ref="F16:H19"/>
+    <mergeCell ref="I16:K19"/>
+    <mergeCell ref="L16:N19"/>
+    <mergeCell ref="O16:Q19"/>
     <mergeCell ref="AM1:AO4"/>
     <mergeCell ref="AM11:AO14"/>
     <mergeCell ref="R1:T4"/>
     <mergeCell ref="R6:T9"/>
     <mergeCell ref="R11:T14"/>
-    <mergeCell ref="C16:E19"/>
-    <mergeCell ref="F16:H19"/>
-    <mergeCell ref="I16:K19"/>
-    <mergeCell ref="L16:N19"/>
-    <mergeCell ref="O16:Q19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2235,12 +2255,12 @@
       <selection activeCell="Z8" sqref="Z8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="4.77734375" customWidth="1"/>
+    <col min="1" max="20" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2274,13 +2294,13 @@
         <v>0</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="2">
-        <v>3</v>
-      </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R1" s="6">
+        <v>3</v>
+      </c>
+      <c r="S1" s="7"/>
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2320,11 +2340,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R2" s="9"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2364,11 +2384,11 @@
         <v>10</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2400,11 +2420,11 @@
         <v>11</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="10"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R4" s="12"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -2448,7 +2468,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>1</v>
       </c>
@@ -2498,7 +2518,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
@@ -2540,7 +2560,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2613,12 +2633,12 @@
       <selection sqref="A1:T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="4.77734375" customWidth="1"/>
+    <col min="1" max="20" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -2662,13 +2682,13 @@
         <v>36</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="2">
-        <v>3</v>
-      </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R1" s="6">
+        <v>3</v>
+      </c>
+      <c r="S1" s="7"/>
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -2712,11 +2732,11 @@
         <v>36</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R2" s="9"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -2750,11 +2770,11 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2792,11 +2812,11 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="10"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R4" s="12"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -2850,7 +2870,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>37</v>
       </c>
@@ -2904,7 +2924,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
@@ -2948,7 +2968,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -3012,12 +3032,12 @@
       <selection activeCell="Z13" sqref="Z13:Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="20" width="4.77734375" customWidth="1"/>
+    <col min="1" max="20" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -3059,13 +3079,13 @@
         <v>44</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="2">
-        <v>3</v>
-      </c>
-      <c r="S1" s="3"/>
-      <c r="T1" s="4"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R1" s="6">
+        <v>3</v>
+      </c>
+      <c r="S1" s="7"/>
+      <c r="T1" s="8"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3105,11 +3125,11 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R2" s="9"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="11"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3149,11 +3169,11 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R3" s="9"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="11"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3195,11 +3215,11 @@
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="8"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="10"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="R4" s="12"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="14"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -3251,7 +3271,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -3301,7 +3321,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -3351,7 +3371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -3421,107 +3441,107 @@
       <selection sqref="A1:T4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="11"/>
-      <c r="C1" s="12">
-        <v>1</v>
-      </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12">
-        <v>0</v>
-      </c>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12">
+      <c r="B1" s="2"/>
+      <c r="C1" s="25">
+        <v>1</v>
+      </c>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25">
+        <v>0</v>
+      </c>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25">
         <v>5</v>
       </c>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12">
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25">
         <v>5</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12">
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25">
         <v>4</v>
       </c>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="11"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
-      <c r="I3" s="12"/>
-      <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="12"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+      <c r="K3" s="25"/>
+      <c r="L3" s="25"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="12"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="25"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
@@ -3573,7 +3593,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
@@ -3625,7 +3645,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
@@ -3677,7 +3697,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">

</xml_diff>

<commit_message>
added shutdownLED back in and did tweaking to Brake Bias
</commit_message>
<xml_diff>
--- a/DIC_doc.xlsx
+++ b/DIC_doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Technik\Technik 2020\04 - Electronics\13 - Software\DIC_Firmware_2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A197AD1-4476-4E62-A5DF-8277D478717D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646517C5-F286-44B0-8BCE-B62FA496AB64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -260,7 +260,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -282,6 +282,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0057A1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color rgb="FF0057A1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -298,7 +312,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.14999847407452621"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,13 +428,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,37 +455,44 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -487,6 +501,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0057A1"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -936,1314 +955,1316 @@
   <dimension ref="A1:AP19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="AL3" sqref="AL3"/>
+      <selection activeCell="AK17" sqref="AK17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="42" width="3.28515625" customWidth="1"/>
+    <col min="1" max="20" width="2.85546875" customWidth="1"/>
+    <col min="21" max="42" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1">
-        <v>1</v>
-      </c>
-      <c r="M1" s="1">
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14">
+        <v>1</v>
+      </c>
+      <c r="M1" s="14">
         <v>2</v>
       </c>
-      <c r="N1" s="1">
-        <v>1</v>
-      </c>
-      <c r="O1" s="1"/>
-      <c r="P1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="6">
-        <v>3</v>
-      </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="5"/>
-      <c r="V1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="N1" s="14">
+        <v>1</v>
+      </c>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="15">
+        <v>3</v>
+      </c>
+      <c r="S1" s="16"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="X1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
-      <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
-      <c r="AG1" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH1" s="1">
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH1" s="14">
         <v>2</v>
       </c>
-      <c r="AI1" s="1">
-        <v>1</v>
-      </c>
-      <c r="AJ1" s="1"/>
-      <c r="AK1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL1" s="1"/>
-      <c r="AM1" s="6">
-        <v>3</v>
-      </c>
-      <c r="AN1" s="7"/>
-      <c r="AO1" s="8"/>
-      <c r="AP1" s="3"/>
-    </row>
-    <row r="2" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="AI1" s="14">
+        <v>1</v>
+      </c>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="15">
+        <v>3</v>
+      </c>
+      <c r="AN1" s="16"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="13"/>
+    </row>
+    <row r="2" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1">
+      <c r="D2" s="14"/>
+      <c r="E2" s="14">
         <v>5</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="14">
         <v>6</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1">
-        <v>1</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1</v>
-      </c>
-      <c r="N2" s="1">
-        <v>3</v>
-      </c>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="X2" s="1" t="s">
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14">
+        <v>1</v>
+      </c>
+      <c r="M2" s="14">
+        <v>1</v>
+      </c>
+      <c r="N2" s="14">
+        <v>3</v>
+      </c>
+      <c r="O2" s="14"/>
+      <c r="P2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1">
+      <c r="Y2" s="14"/>
+      <c r="Z2" s="14">
         <v>5</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AA2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB2" s="14">
         <v>6</v>
       </c>
-      <c r="AC2" s="1" t="s">
+      <c r="AC2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="AD2" s="1"/>
-      <c r="AE2" s="1"/>
-      <c r="AF2" s="1"/>
-      <c r="AG2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AJ2" s="1"/>
-      <c r="AK2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="1"/>
-      <c r="AM2" s="9"/>
-      <c r="AN2" s="10"/>
-      <c r="AO2" s="11"/>
-      <c r="AP2" s="3"/>
-    </row>
-    <row r="3" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="AD2" s="14"/>
+      <c r="AE2" s="14"/>
+      <c r="AF2" s="14"/>
+      <c r="AG2" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH2" s="14">
+        <v>1</v>
+      </c>
+      <c r="AI2" s="14">
+        <v>3</v>
+      </c>
+      <c r="AJ2" s="14"/>
+      <c r="AK2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="14"/>
+      <c r="AM2" s="19"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="21"/>
+      <c r="AP2" s="13"/>
+    </row>
+    <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1">
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14">
         <v>5</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" s="14">
         <v>6</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="1" t="s">
+      <c r="G3" s="14"/>
+      <c r="H3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="K3" s="14"/>
+      <c r="L3" s="14">
+        <v>1</v>
+      </c>
+      <c r="M3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="1">
+      <c r="N3" s="14">
         <v>5</v>
       </c>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1" t="s">
+      <c r="O3" s="14"/>
+      <c r="P3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="1" t="s">
+      <c r="Q3" s="14"/>
+      <c r="R3" s="19"/>
+      <c r="S3" s="20"/>
+      <c r="T3" s="21"/>
+      <c r="U3" s="18"/>
+      <c r="V3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="W3" s="1" t="s">
+      <c r="W3" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="X3" s="1"/>
-      <c r="Y3" s="1"/>
-      <c r="Z3" s="1">
+      <c r="X3" s="14"/>
+      <c r="Y3" s="14"/>
+      <c r="Z3" s="14">
         <v>5</v>
       </c>
-      <c r="AA3" s="1">
+      <c r="AA3" s="14">
         <v>6</v>
       </c>
-      <c r="AB3" s="1"/>
-      <c r="AC3" s="1" t="s">
+      <c r="AB3" s="14"/>
+      <c r="AC3" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="AD3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="1"/>
-      <c r="AF3" s="1" t="s">
+      <c r="AD3" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="14"/>
+      <c r="AF3" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="AG3" s="1" t="s">
+      <c r="AG3" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AH3" s="1" t="s">
+      <c r="AH3" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="AI3" s="1" t="s">
+      <c r="AI3" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="AJ3" s="1" t="s">
+      <c r="AJ3" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="AK3" s="1" t="s">
+      <c r="AK3" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="AL3" s="1"/>
-      <c r="AM3" s="9"/>
-      <c r="AN3" s="10"/>
-      <c r="AO3" s="11"/>
-      <c r="AP3" s="3"/>
-    </row>
-    <row r="4" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="AL3" s="14"/>
+      <c r="AM3" s="19"/>
+      <c r="AN3" s="20"/>
+      <c r="AO3" s="21"/>
+      <c r="AP3" s="13"/>
+    </row>
+    <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14">
+        <v>1</v>
+      </c>
+      <c r="L4" s="14">
         <v>2</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="M4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="N4" s="1">
+      <c r="N4" s="14">
         <v>4</v>
       </c>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1" t="s">
+      <c r="O4" s="14"/>
+      <c r="P4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="1"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4" t="s">
+      <c r="Q4" s="14"/>
+      <c r="R4" s="22"/>
+      <c r="S4" s="23"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="18"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="Y4" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="4" t="s">
+      <c r="Y4" s="14">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AA4" s="4">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="4">
+      <c r="AA4" s="14">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="14">
         <v>4</v>
       </c>
-      <c r="AC4" s="4">
+      <c r="AC4" s="14">
         <v>2</v>
       </c>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="1"/>
-      <c r="AF4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="1">
+      <c r="AD4" s="14"/>
+      <c r="AE4" s="14"/>
+      <c r="AF4" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="14">
         <v>2</v>
       </c>
-      <c r="AH4" s="1" t="s">
+      <c r="AH4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="AI4" s="1">
+      <c r="AI4" s="14">
         <v>4</v>
       </c>
-      <c r="AJ4" s="1"/>
-      <c r="AK4" s="1" t="s">
+      <c r="AJ4" s="14"/>
+      <c r="AK4" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="AL4" s="1"/>
-      <c r="AM4" s="12"/>
-      <c r="AN4" s="13"/>
-      <c r="AO4" s="14"/>
-      <c r="AP4" s="3"/>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="5"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AJ5" s="3"/>
-      <c r="AK5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AM5" s="3"/>
-      <c r="AN5" s="3"/>
-      <c r="AO5" s="3"/>
-      <c r="AP5" s="3"/>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="AL4" s="14"/>
+      <c r="AM4" s="22"/>
+      <c r="AN4" s="23"/>
+      <c r="AO4" s="24"/>
+      <c r="AP4" s="13"/>
+    </row>
+    <row r="5" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
+      <c r="K5" s="18"/>
+      <c r="L5" s="18"/>
+      <c r="M5" s="18"/>
+      <c r="N5" s="18"/>
+      <c r="O5" s="18"/>
+      <c r="P5" s="18"/>
+      <c r="Q5" s="18"/>
+      <c r="R5" s="18"/>
+      <c r="S5" s="18"/>
+      <c r="T5" s="18"/>
+      <c r="U5" s="18"/>
+      <c r="V5" s="18"/>
+      <c r="W5" s="18"/>
+      <c r="X5" s="18"/>
+      <c r="Y5" s="18"/>
+      <c r="Z5" s="18"/>
+      <c r="AA5" s="18"/>
+      <c r="AB5" s="18"/>
+      <c r="AC5" s="18"/>
+      <c r="AD5" s="18"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="18"/>
+      <c r="AG5" s="18"/>
+      <c r="AH5" s="18"/>
+      <c r="AI5" s="18"/>
+      <c r="AJ5" s="18"/>
+      <c r="AK5" s="18"/>
+      <c r="AL5" s="18"/>
+      <c r="AM5" s="18"/>
+      <c r="AN5" s="18"/>
+      <c r="AO5" s="18"/>
+      <c r="AP5" s="13"/>
+    </row>
+    <row r="6" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4">
-        <v>1</v>
-      </c>
-      <c r="G6" s="4">
-        <v>0</v>
-      </c>
-      <c r="H6" s="4">
-        <v>0</v>
-      </c>
-      <c r="I6" s="4" t="s">
+      <c r="D6" s="14">
+        <v>1</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14">
+        <v>1</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0</v>
+      </c>
+      <c r="I6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4">
+      <c r="J6" s="14"/>
+      <c r="K6" s="14">
         <v>2</v>
       </c>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4">
-        <v>1</v>
-      </c>
-      <c r="N6" s="4">
-        <v>0</v>
-      </c>
-      <c r="O6" s="4">
-        <v>0</v>
-      </c>
-      <c r="P6" s="4" t="s">
+      <c r="L6" s="14"/>
+      <c r="M6" s="14">
+        <v>1</v>
+      </c>
+      <c r="N6" s="14">
+        <v>0</v>
+      </c>
+      <c r="O6" s="14">
+        <v>0</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="Q6" s="4"/>
+      <c r="Q6" s="14"/>
       <c r="R6" s="15">
         <v>3</v>
       </c>
       <c r="S6" s="16"/>
       <c r="T6" s="17"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
-      <c r="Z6" s="3"/>
-      <c r="AA6" s="3"/>
-      <c r="AB6" s="3"/>
-      <c r="AC6" s="3"/>
-      <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AJ6" s="3"/>
-      <c r="AK6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AM6" s="3"/>
-      <c r="AN6" s="3"/>
-      <c r="AO6" s="3"/>
-      <c r="AP6" s="3"/>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="18"/>
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+      <c r="AL6" s="18"/>
+      <c r="AM6" s="18"/>
+      <c r="AN6" s="18"/>
+      <c r="AO6" s="18"/>
+      <c r="AP6" s="13"/>
+    </row>
+    <row r="7" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4">
-        <v>1</v>
-      </c>
-      <c r="G7" s="4">
-        <v>0</v>
-      </c>
-      <c r="H7" s="4">
-        <v>0</v>
-      </c>
-      <c r="I7" s="4" t="s">
+      <c r="D7" s="14">
+        <v>1</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14">
+        <v>1</v>
+      </c>
+      <c r="G7" s="14">
+        <v>0</v>
+      </c>
+      <c r="H7" s="14">
+        <v>0</v>
+      </c>
+      <c r="I7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4">
+      <c r="J7" s="14"/>
+      <c r="K7" s="14">
         <v>2</v>
       </c>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4">
-        <v>1</v>
-      </c>
-      <c r="N7" s="4">
-        <v>0</v>
-      </c>
-      <c r="O7" s="4">
-        <v>0</v>
-      </c>
-      <c r="P7" s="4" t="s">
+      <c r="L7" s="14"/>
+      <c r="M7" s="14">
+        <v>1</v>
+      </c>
+      <c r="N7" s="14">
+        <v>0</v>
+      </c>
+      <c r="O7" s="14">
+        <v>0</v>
+      </c>
+      <c r="P7" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="Q7" s="4"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="19"/>
-      <c r="T7" s="20"/>
-      <c r="U7" s="5"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3"/>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-      <c r="AK7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AM7" s="3"/>
-      <c r="AN7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AP7" s="3"/>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="Q7" s="14"/>
+      <c r="R7" s="19"/>
+      <c r="S7" s="20"/>
+      <c r="T7" s="21"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+      <c r="AL7" s="18"/>
+      <c r="AM7" s="18"/>
+      <c r="AN7" s="18"/>
+      <c r="AO7" s="18"/>
+      <c r="AP7" s="13"/>
+    </row>
+    <row r="8" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4">
-        <v>1</v>
-      </c>
-      <c r="G8" s="4">
-        <v>0</v>
-      </c>
-      <c r="H8" s="4">
-        <v>0</v>
-      </c>
-      <c r="I8" s="4" t="s">
+      <c r="D8" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="14"/>
+      <c r="F8" s="14">
+        <v>1</v>
+      </c>
+      <c r="G8" s="14">
+        <v>0</v>
+      </c>
+      <c r="H8" s="14">
+        <v>0</v>
+      </c>
+      <c r="I8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="19"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AJ8" s="3"/>
-      <c r="AK8" s="3"/>
-      <c r="AL8" s="3"/>
-      <c r="AM8" s="3"/>
-      <c r="AN8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AP8" s="3"/>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="19"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="21"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="18"/>
+      <c r="AM8" s="18"/>
+      <c r="AN8" s="18"/>
+      <c r="AO8" s="18"/>
+      <c r="AP8" s="13"/>
+    </row>
+    <row r="9" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4">
-        <v>9</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="4" t="s">
+      <c r="D9" s="14"/>
+      <c r="E9" s="14">
+        <v>9</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
+      <c r="H9" s="14"/>
+      <c r="I9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4">
-        <v>9</v>
-      </c>
-      <c r="L9" s="4">
-        <v>0</v>
-      </c>
-      <c r="M9" s="4" t="s">
+      <c r="J9" s="14"/>
+      <c r="K9" s="14">
+        <v>9</v>
+      </c>
+      <c r="L9" s="14">
+        <v>0</v>
+      </c>
+      <c r="M9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="21"/>
-      <c r="S9" s="22"/>
-      <c r="T9" s="23"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
-      <c r="AF9" s="3"/>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
-      <c r="AJ9" s="3"/>
-      <c r="AK9" s="3"/>
-      <c r="AL9" s="3"/>
-      <c r="AM9" s="3"/>
-      <c r="AN9" s="3"/>
-      <c r="AO9" s="3"/>
-      <c r="AP9" s="3"/>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-      <c r="S10" s="5"/>
-      <c r="T10" s="5"/>
-      <c r="U10" s="5"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
-      <c r="Z10" s="3"/>
-      <c r="AA10" s="3"/>
-      <c r="AB10" s="3"/>
-      <c r="AC10" s="3"/>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3"/>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
-      <c r="AJ10" s="3"/>
-      <c r="AK10" s="3"/>
-      <c r="AL10" s="3"/>
-      <c r="AM10" s="3"/>
-      <c r="AN10" s="3"/>
-      <c r="AO10" s="3"/>
-      <c r="AP10" s="3"/>
-    </row>
-    <row r="11" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="22"/>
+      <c r="S9" s="23"/>
+      <c r="T9" s="24"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="18"/>
+      <c r="AM9" s="18"/>
+      <c r="AN9" s="18"/>
+      <c r="AO9" s="18"/>
+      <c r="AP9" s="13"/>
+    </row>
+    <row r="10" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="18"/>
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="18"/>
+      <c r="AI10" s="18"/>
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+      <c r="AL10" s="18"/>
+      <c r="AM10" s="18"/>
+      <c r="AN10" s="18"/>
+      <c r="AO10" s="18"/>
+      <c r="AP10" s="13"/>
+    </row>
+    <row r="11" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4">
-        <v>9</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4" t="s">
+      <c r="B11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14">
+        <v>9</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="H11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4">
-        <v>1</v>
-      </c>
-      <c r="L11" s="4">
-        <v>1</v>
-      </c>
-      <c r="M11" s="4">
+      <c r="I11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14">
+        <v>1</v>
+      </c>
+      <c r="L11" s="14">
+        <v>1</v>
+      </c>
+      <c r="M11" s="14">
         <v>2</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="N11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="O11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="P11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="Q11" s="4"/>
+      <c r="Q11" s="14"/>
       <c r="R11" s="15">
         <v>3</v>
       </c>
       <c r="S11" s="16"/>
       <c r="T11" s="17"/>
-      <c r="U11" s="5"/>
-      <c r="V11" s="4" t="s">
+      <c r="U11" s="18"/>
+      <c r="V11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="W11" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4">
-        <v>9</v>
-      </c>
-      <c r="Z11" s="4"/>
-      <c r="AA11" s="4"/>
-      <c r="AB11" s="4" t="s">
+      <c r="W11" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14">
+        <v>9</v>
+      </c>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AC11" s="4" t="s">
+      <c r="AC11" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="AD11" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="AE11" s="4"/>
-      <c r="AF11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG11" s="4">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="4">
+      <c r="AD11" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AE11" s="14"/>
+      <c r="AF11" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG11" s="14">
+        <v>1</v>
+      </c>
+      <c r="AH11" s="14">
         <v>2</v>
       </c>
-      <c r="AI11" s="4" t="s">
+      <c r="AI11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AJ11" s="4" t="s">
+      <c r="AJ11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AK11" s="4" t="s">
+      <c r="AK11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="AL11" s="4"/>
+      <c r="AL11" s="14"/>
       <c r="AM11" s="15">
         <v>3</v>
       </c>
       <c r="AN11" s="16"/>
       <c r="AO11" s="17"/>
-      <c r="AP11" s="3"/>
-    </row>
-    <row r="12" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="AP11" s="13"/>
+    </row>
+    <row r="12" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="4" t="s">
+      <c r="B12" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4">
-        <v>1</v>
-      </c>
-      <c r="F12" s="4" t="s">
+      <c r="D12" s="14"/>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="4">
-        <v>1</v>
-      </c>
-      <c r="H12" s="4">
-        <v>3</v>
-      </c>
-      <c r="I12" s="4" t="s">
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+      <c r="H12" s="14">
+        <v>3</v>
+      </c>
+      <c r="I12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="14">
         <v>4</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="14">
         <v>5</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="14">
         <v>6</v>
       </c>
-      <c r="M12" s="4"/>
-      <c r="N12" s="4"/>
-      <c r="O12" s="4"/>
-      <c r="P12" s="4"/>
-      <c r="Q12" s="4"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="19"/>
-      <c r="T12" s="20"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="4" t="s">
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="19"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="W12" s="4" t="s">
+      <c r="W12" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="X12" s="4" t="s">
+      <c r="X12" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="Y12" s="4"/>
-      <c r="Z12" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="4" t="s">
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AB12" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="4">
-        <v>3</v>
-      </c>
-      <c r="AD12" s="4" t="s">
+      <c r="AB12" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="14">
+        <v>3</v>
+      </c>
+      <c r="AD12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AE12" s="4">
+      <c r="AE12" s="14">
         <v>4</v>
       </c>
-      <c r="AF12" s="4">
+      <c r="AF12" s="14">
         <v>5</v>
       </c>
-      <c r="AG12" s="4">
+      <c r="AG12" s="14">
         <v>6</v>
       </c>
-      <c r="AH12" s="4"/>
-      <c r="AI12" s="4"/>
-      <c r="AJ12" s="4"/>
-      <c r="AK12" s="4"/>
-      <c r="AL12" s="4"/>
-      <c r="AM12" s="18"/>
-      <c r="AN12" s="19"/>
-      <c r="AO12" s="20"/>
-      <c r="AP12" s="3"/>
-    </row>
-    <row r="13" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="AH12" s="14"/>
+      <c r="AI12" s="14"/>
+      <c r="AJ12" s="14"/>
+      <c r="AK12" s="14"/>
+      <c r="AL12" s="14"/>
+      <c r="AM12" s="19"/>
+      <c r="AN12" s="20"/>
+      <c r="AO12" s="21"/>
+      <c r="AP12" s="13"/>
+    </row>
+    <row r="13" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4" t="s">
+      <c r="C13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14">
+        <v>1</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G13" s="4">
-        <v>1</v>
-      </c>
-      <c r="H13" s="4">
+      <c r="G13" s="14">
+        <v>1</v>
+      </c>
+      <c r="H13" s="14">
         <v>4</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="I13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="14">
         <v>6</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="14">
         <v>7</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="14">
         <v>8</v>
       </c>
-      <c r="M13" s="4"/>
-      <c r="N13" s="4"/>
-      <c r="O13" s="4"/>
-      <c r="P13" s="4"/>
-      <c r="Q13" s="4"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="19"/>
-      <c r="T13" s="20"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="4" t="s">
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="14"/>
+      <c r="P13" s="14"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="19"/>
+      <c r="S13" s="20"/>
+      <c r="T13" s="21"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="W13" s="4" t="s">
+      <c r="W13" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="X13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y13" s="4"/>
-      <c r="Z13" s="4">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="4" t="s">
+      <c r="X13" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y13" s="14"/>
+      <c r="Z13" s="14">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AB13" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC13" s="4">
+      <c r="AB13" s="14">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="14">
         <v>4</v>
       </c>
-      <c r="AD13" s="4" t="s">
+      <c r="AD13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="AE13" s="4">
+      <c r="AE13" s="14">
         <v>6</v>
       </c>
-      <c r="AF13" s="4">
+      <c r="AF13" s="14">
         <v>7</v>
       </c>
-      <c r="AG13" s="4">
+      <c r="AG13" s="14">
         <v>8</v>
       </c>
-      <c r="AH13" s="4"/>
-      <c r="AI13" s="4"/>
-      <c r="AJ13" s="4"/>
-      <c r="AK13" s="4"/>
-      <c r="AL13" s="4"/>
-      <c r="AM13" s="18"/>
-      <c r="AN13" s="19"/>
-      <c r="AO13" s="20"/>
-      <c r="AP13" s="3"/>
-    </row>
-    <row r="14" spans="1:42" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="AH13" s="14"/>
+      <c r="AI13" s="14"/>
+      <c r="AJ13" s="14"/>
+      <c r="AK13" s="14"/>
+      <c r="AL13" s="14"/>
+      <c r="AM13" s="19"/>
+      <c r="AN13" s="20"/>
+      <c r="AO13" s="21"/>
+      <c r="AP13" s="13"/>
+    </row>
+    <row r="14" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
-        <v>3</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="C14" s="14"/>
+      <c r="D14" s="14">
+        <v>3</v>
+      </c>
+      <c r="E14" s="14">
         <v>4</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="H14" s="4" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="I14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4">
-        <v>1</v>
-      </c>
-      <c r="L14" s="4">
-        <v>3</v>
-      </c>
-      <c r="M14" s="4">
-        <v>9</v>
-      </c>
-      <c r="N14" s="4" t="s">
+      <c r="I14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14">
+        <v>1</v>
+      </c>
+      <c r="L14" s="14">
+        <v>3</v>
+      </c>
+      <c r="M14" s="14">
+        <v>9</v>
+      </c>
+      <c r="N14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="O14" s="4" t="s">
+      <c r="O14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="21"/>
-      <c r="S14" s="22"/>
-      <c r="T14" s="23"/>
-      <c r="U14" s="5"/>
-      <c r="V14" s="4" t="s">
+      <c r="P14" s="14"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="22"/>
+      <c r="S14" s="23"/>
+      <c r="T14" s="24"/>
+      <c r="U14" s="18"/>
+      <c r="V14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="W14" s="4" t="s">
+      <c r="W14" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4">
-        <v>3</v>
-      </c>
-      <c r="Z14" s="4">
+      <c r="X14" s="14"/>
+      <c r="Y14" s="14">
+        <v>3</v>
+      </c>
+      <c r="Z14" s="14">
         <v>4</v>
       </c>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AC14" s="4" t="s">
+      <c r="AA14" s="14"/>
+      <c r="AB14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC14" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="AD14" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="AE14" s="4"/>
-      <c r="AF14" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG14" s="4">
-        <v>3</v>
-      </c>
-      <c r="AH14" s="4">
-        <v>9</v>
-      </c>
-      <c r="AI14" s="4" t="s">
+      <c r="AD14" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="14"/>
+      <c r="AF14" s="14">
+        <v>1</v>
+      </c>
+      <c r="AG14" s="14">
+        <v>3</v>
+      </c>
+      <c r="AH14" s="14">
+        <v>9</v>
+      </c>
+      <c r="AI14" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="AJ14" s="4" t="s">
+      <c r="AJ14" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="AK14" s="4"/>
-      <c r="AL14" s="4"/>
-      <c r="AM14" s="21"/>
-      <c r="AN14" s="22"/>
-      <c r="AO14" s="23"/>
-      <c r="AP14" s="3"/>
-    </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
-      <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="5"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="5"/>
-      <c r="R15" s="5"/>
-      <c r="S15" s="5"/>
-      <c r="T15" s="5"/>
-      <c r="U15" s="5"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
-      <c r="Z15" s="3"/>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3"/>
-      <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
-      <c r="AI15" s="3"/>
-      <c r="AJ15" s="3"/>
-      <c r="AK15" s="3"/>
-      <c r="AL15" s="3"/>
-      <c r="AM15" s="3"/>
-      <c r="AN15" s="3"/>
-      <c r="AO15" s="3"/>
-      <c r="AP15" s="3"/>
-    </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="24">
-        <v>1</v>
-      </c>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24">
-        <v>0</v>
-      </c>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24">
+      <c r="AK14" s="14"/>
+      <c r="AL14" s="14"/>
+      <c r="AM14" s="22"/>
+      <c r="AN14" s="23"/>
+      <c r="AO14" s="24"/>
+      <c r="AP14" s="13"/>
+    </row>
+    <row r="15" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="18"/>
+      <c r="O15" s="18"/>
+      <c r="P15" s="18"/>
+      <c r="Q15" s="18"/>
+      <c r="R15" s="18"/>
+      <c r="S15" s="18"/>
+      <c r="T15" s="18"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="18"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="18"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+      <c r="AL15" s="18"/>
+      <c r="AM15" s="18"/>
+      <c r="AN15" s="18"/>
+      <c r="AO15" s="18"/>
+      <c r="AP15" s="13"/>
+    </row>
+    <row r="16" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="25">
+        <v>1</v>
+      </c>
+      <c r="D16" s="25"/>
+      <c r="E16" s="25"/>
+      <c r="F16" s="25">
+        <v>0</v>
+      </c>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
+      <c r="I16" s="25">
         <v>5</v>
       </c>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24">
+      <c r="J16" s="25"/>
+      <c r="K16" s="25"/>
+      <c r="L16" s="25">
         <v>5</v>
       </c>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-      <c r="O16" s="24">
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25">
         <v>4</v>
       </c>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="4"/>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3"/>
-      <c r="AA16" s="3"/>
-      <c r="AB16" s="3"/>
-      <c r="AC16" s="3"/>
-      <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
-      <c r="AF16" s="3"/>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
-      <c r="AJ16" s="3"/>
-      <c r="AK16" s="3"/>
-      <c r="AL16" s="3"/>
-      <c r="AM16" s="3"/>
-      <c r="AN16" s="3"/>
-      <c r="AO16" s="3"/>
-      <c r="AP16" s="3"/>
-    </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="24"/>
-      <c r="N17" s="24"/>
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="4"/>
-      <c r="S17" s="4"/>
-      <c r="T17" s="4"/>
-      <c r="U17" s="5"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
-      <c r="Z17" s="3"/>
-      <c r="AA17" s="3"/>
-      <c r="AB17" s="3"/>
-      <c r="AC17" s="3"/>
-      <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
-      <c r="AF17" s="3"/>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
-      <c r="AJ17" s="3"/>
-      <c r="AK17" s="3"/>
-      <c r="AL17" s="3"/>
-      <c r="AM17" s="3"/>
-      <c r="AN17" s="3"/>
-      <c r="AO17" s="3"/>
-      <c r="AP17" s="3"/>
-    </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="24"/>
-      <c r="H18" s="24"/>
-      <c r="I18" s="24"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="24"/>
-      <c r="L18" s="24"/>
-      <c r="M18" s="24"/>
-      <c r="N18" s="24"/>
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="5"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
-      <c r="Z18" s="3"/>
-      <c r="AA18" s="3"/>
-      <c r="AB18" s="3"/>
-      <c r="AC18" s="3"/>
-      <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
-      <c r="AF18" s="3"/>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
-      <c r="AJ18" s="3"/>
-      <c r="AK18" s="3"/>
-      <c r="AL18" s="3"/>
-      <c r="AM18" s="3"/>
-      <c r="AN18" s="3"/>
-      <c r="AO18" s="3"/>
-      <c r="AP18" s="3"/>
-    </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="24"/>
-      <c r="F19" s="24"/>
-      <c r="G19" s="24"/>
-      <c r="H19" s="24"/>
-      <c r="I19" s="24"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="24"/>
-      <c r="L19" s="24"/>
-      <c r="M19" s="24"/>
-      <c r="N19" s="24"/>
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="4"/>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4"/>
-      <c r="U19" s="5"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
-      <c r="Z19" s="3"/>
-      <c r="AA19" s="3"/>
-      <c r="AB19" s="3"/>
-      <c r="AC19" s="3"/>
-      <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
-      <c r="AF19" s="3"/>
-      <c r="AG19" s="3"/>
-      <c r="AH19" s="3"/>
-      <c r="AI19" s="3"/>
-      <c r="AJ19" s="3"/>
-      <c r="AK19" s="3"/>
-      <c r="AL19" s="3"/>
-      <c r="AM19" s="3"/>
-      <c r="AN19" s="3"/>
-      <c r="AO19" s="3"/>
-      <c r="AP19" s="3"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="18"/>
+      <c r="AI16" s="18"/>
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+      <c r="AL16" s="18"/>
+      <c r="AM16" s="18"/>
+      <c r="AN16" s="18"/>
+      <c r="AO16" s="18"/>
+      <c r="AP16" s="13"/>
+    </row>
+    <row r="17" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="25"/>
+      <c r="E17" s="25"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="25"/>
+      <c r="K17" s="25"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="18"/>
+      <c r="V17" s="18"/>
+      <c r="W17" s="18"/>
+      <c r="X17" s="18"/>
+      <c r="Y17" s="18"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="18"/>
+      <c r="AG17" s="18"/>
+      <c r="AH17" s="18"/>
+      <c r="AI17" s="18"/>
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+      <c r="AL17" s="18"/>
+      <c r="AM17" s="18"/>
+      <c r="AN17" s="18"/>
+      <c r="AO17" s="18"/>
+      <c r="AP17" s="13"/>
+    </row>
+    <row r="18" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="25"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
+      <c r="I18" s="25"/>
+      <c r="J18" s="25"/>
+      <c r="K18" s="25"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="14"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="18"/>
+      <c r="V18" s="18"/>
+      <c r="W18" s="18"/>
+      <c r="X18" s="18"/>
+      <c r="Y18" s="18"/>
+      <c r="Z18" s="18"/>
+      <c r="AA18" s="18"/>
+      <c r="AB18" s="18"/>
+      <c r="AC18" s="18"/>
+      <c r="AD18" s="18"/>
+      <c r="AE18" s="18"/>
+      <c r="AF18" s="18"/>
+      <c r="AG18" s="18"/>
+      <c r="AH18" s="18"/>
+      <c r="AI18" s="18"/>
+      <c r="AJ18" s="18"/>
+      <c r="AK18" s="18"/>
+      <c r="AL18" s="18"/>
+      <c r="AM18" s="18"/>
+      <c r="AN18" s="18"/>
+      <c r="AO18" s="18"/>
+      <c r="AP18" s="13"/>
+    </row>
+    <row r="19" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="25"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="25"/>
+      <c r="F19" s="25"/>
+      <c r="G19" s="25"/>
+      <c r="H19" s="25"/>
+      <c r="I19" s="25"/>
+      <c r="J19" s="25"/>
+      <c r="K19" s="25"/>
+      <c r="L19" s="25"/>
+      <c r="M19" s="25"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="25"/>
+      <c r="P19" s="25"/>
+      <c r="Q19" s="25"/>
+      <c r="R19" s="14"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="18"/>
+      <c r="V19" s="18"/>
+      <c r="W19" s="18"/>
+      <c r="X19" s="18"/>
+      <c r="Y19" s="18"/>
+      <c r="Z19" s="18"/>
+      <c r="AA19" s="18"/>
+      <c r="AB19" s="18"/>
+      <c r="AC19" s="18"/>
+      <c r="AD19" s="18"/>
+      <c r="AE19" s="18"/>
+      <c r="AF19" s="18"/>
+      <c r="AG19" s="18"/>
+      <c r="AH19" s="18"/>
+      <c r="AI19" s="18"/>
+      <c r="AJ19" s="18"/>
+      <c r="AK19" s="18"/>
+      <c r="AL19" s="18"/>
+      <c r="AM19" s="18"/>
+      <c r="AN19" s="18"/>
+      <c r="AO19" s="18"/>
+      <c r="AP19" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AM1:AO4"/>
+    <mergeCell ref="AM11:AO14"/>
+    <mergeCell ref="R1:T4"/>
+    <mergeCell ref="R6:T9"/>
+    <mergeCell ref="R11:T14"/>
     <mergeCell ref="C16:E19"/>
     <mergeCell ref="F16:H19"/>
     <mergeCell ref="I16:K19"/>
     <mergeCell ref="L16:N19"/>
     <mergeCell ref="O16:Q19"/>
-    <mergeCell ref="AM1:AO4"/>
-    <mergeCell ref="AM11:AO14"/>
-    <mergeCell ref="R1:T4"/>
-    <mergeCell ref="R6:T9"/>
-    <mergeCell ref="R11:T14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2260,7 +2281,7 @@
     <col min="1" max="20" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2294,13 +2315,13 @@
         <v>0</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="6">
-        <v>3</v>
-      </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="8"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R1" s="3">
+        <v>3</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -2340,11 +2361,11 @@
         <v>0</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R2" s="6"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2384,11 +2405,11 @@
         <v>10</v>
       </c>
       <c r="Q3" s="1"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="11"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R3" s="6"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2420,9 +2441,9 @@
         <v>11</v>
       </c>
       <c r="Q4" s="1"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="14"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="11"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2638,7 +2659,7 @@
     <col min="1" max="20" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -2682,13 +2703,13 @@
         <v>36</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="6">
-        <v>3</v>
-      </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="8"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R1" s="3">
+        <v>3</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>37</v>
       </c>
@@ -2732,11 +2753,11 @@
         <v>36</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R2" s="6"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>33</v>
       </c>
@@ -2770,11 +2791,11 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="11"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R3" s="6"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -2812,9 +2833,9 @@
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="14"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="11"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -3037,7 +3058,7 @@
     <col min="1" max="20" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>33</v>
       </c>
@@ -3079,13 +3100,13 @@
         <v>44</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="6">
-        <v>3</v>
-      </c>
-      <c r="S1" s="7"/>
-      <c r="T1" s="8"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R1" s="3">
+        <v>3</v>
+      </c>
+      <c r="S1" s="4"/>
+      <c r="T1" s="5"/>
+    </row>
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -3125,11 +3146,11 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="9"/>
-      <c r="S2" s="10"/>
-      <c r="T2" s="11"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R2" s="6"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="8"/>
+    </row>
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -3169,11 +3190,11 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="9"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="11"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="R3" s="6"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="8"/>
+    </row>
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -3215,9 +3236,9 @@
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="12"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="14"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="11"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -3443,100 +3464,100 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="25">
-        <v>1</v>
-      </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25">
-        <v>0</v>
-      </c>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25">
+      <c r="C1" s="12">
+        <v>1</v>
+      </c>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12">
+        <v>0</v>
+      </c>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12">
         <v>5</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25">
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12">
         <v>5</v>
       </c>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25">
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12">
         <v>4</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
       <c r="R1" s="2"/>
       <c r="S1" s="2"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="25"/>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="25"/>
-      <c r="M2" s="25"/>
-      <c r="N2" s="25"/>
-      <c r="O2" s="25"/>
-      <c r="P2" s="25"/>
-      <c r="Q2" s="25"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
       <c r="R2" s="2"/>
       <c r="S2" s="2"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="2"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="25"/>
-      <c r="M4" s="25"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
-      <c r="P4" s="25"/>
-      <c r="Q4" s="25"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
       <c r="T4" s="1"/>

</xml_diff>

<commit_message>
added debug screen functionality
</commit_message>
<xml_diff>
--- a/DIC_doc.xlsx
+++ b/DIC_doc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\DIC_Firmware_legacy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AD3674-A763-4FBE-ABF8-71F07C5FA8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{197A5433-838E-4FBA-A058-AC2A6F985603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="2130" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="98">
   <si>
     <t>C</t>
   </si>
@@ -503,6 +503,75 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -530,9 +599,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,72 +627,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1132,11 +1132,11 @@
         <v>0</v>
       </c>
       <c r="Q1" s="3"/>
-      <c r="R1" s="5">
+      <c r="R1" s="28">
         <v>3</v>
       </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="7"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="30"/>
       <c r="U1" s="4"/>
       <c r="V1" s="3" t="s">
         <v>0</v>
@@ -1171,11 +1171,11 @@
         <v>0</v>
       </c>
       <c r="AL1" s="3"/>
-      <c r="AM1" s="5">
+      <c r="AM1" s="28">
         <v>3</v>
       </c>
-      <c r="AN1" s="6"/>
-      <c r="AO1" s="7"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="30"/>
       <c r="AP1" s="2"/>
     </row>
     <row r="2" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1218,9 +1218,9 @@
         <v>0</v>
       </c>
       <c r="Q2" s="3"/>
-      <c r="R2" s="8"/>
-      <c r="S2" s="9"/>
-      <c r="T2" s="10"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="33"/>
       <c r="U2" s="4"/>
       <c r="V2" s="3" t="s">
         <v>1</v>
@@ -1261,9 +1261,9 @@
         <v>0</v>
       </c>
       <c r="AL2" s="3"/>
-      <c r="AM2" s="8"/>
-      <c r="AN2" s="9"/>
-      <c r="AO2" s="10"/>
+      <c r="AM2" s="31"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="33"/>
       <c r="AP2" s="2"/>
     </row>
     <row r="3" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1306,9 +1306,9 @@
         <v>10</v>
       </c>
       <c r="Q3" s="3"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="10"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="32"/>
+      <c r="T3" s="33"/>
       <c r="U3" s="4"/>
       <c r="V3" s="3" t="s">
         <v>5</v>
@@ -1351,9 +1351,9 @@
         <v>61</v>
       </c>
       <c r="AL3" s="3"/>
-      <c r="AM3" s="8"/>
-      <c r="AN3" s="9"/>
-      <c r="AO3" s="10"/>
+      <c r="AM3" s="31"/>
+      <c r="AN3" s="32"/>
+      <c r="AO3" s="33"/>
       <c r="AP3" s="2"/>
     </row>
     <row r="4" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1388,9 +1388,9 @@
         <v>11</v>
       </c>
       <c r="Q4" s="3"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="12"/>
-      <c r="T4" s="13"/>
+      <c r="R4" s="34"/>
+      <c r="S4" s="35"/>
+      <c r="T4" s="36"/>
       <c r="U4" s="4"/>
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
@@ -1431,9 +1431,9 @@
         <v>11</v>
       </c>
       <c r="AL4" s="3"/>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="12"/>
-      <c r="AO4" s="13"/>
+      <c r="AM4" s="34"/>
+      <c r="AN4" s="35"/>
+      <c r="AO4" s="36"/>
       <c r="AP4" s="2"/>
     </row>
     <row r="5" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1524,11 +1524,11 @@
         <v>23</v>
       </c>
       <c r="Q6" s="3"/>
-      <c r="R6" s="5">
+      <c r="R6" s="28">
         <v>3</v>
       </c>
-      <c r="S6" s="6"/>
-      <c r="T6" s="7"/>
+      <c r="S6" s="29"/>
+      <c r="T6" s="30"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
       <c r="W6" s="4"/>
@@ -1596,9 +1596,9 @@
         <v>23</v>
       </c>
       <c r="Q7" s="3"/>
-      <c r="R7" s="8"/>
-      <c r="S7" s="9"/>
-      <c r="T7" s="10"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="32"/>
+      <c r="T7" s="33"/>
       <c r="U7" s="4"/>
       <c r="V7" s="4"/>
       <c r="W7" s="4"/>
@@ -1656,9 +1656,9 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="R8" s="8"/>
-      <c r="S8" s="9"/>
-      <c r="T8" s="10"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="32"/>
+      <c r="T8" s="33"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
       <c r="W8" s="4"/>
@@ -1720,9 +1720,9 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
       <c r="Q9" s="3"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="12"/>
-      <c r="T9" s="13"/>
+      <c r="R9" s="34"/>
+      <c r="S9" s="35"/>
+      <c r="T9" s="36"/>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
@@ -1832,11 +1832,11 @@
         <v>31</v>
       </c>
       <c r="Q11" s="3"/>
-      <c r="R11" s="5">
+      <c r="R11" s="28">
         <v>3</v>
       </c>
-      <c r="S11" s="6"/>
-      <c r="T11" s="7"/>
+      <c r="S11" s="29"/>
+      <c r="T11" s="30"/>
       <c r="U11" s="4"/>
       <c r="V11" s="3" t="s">
         <v>20</v>
@@ -1879,11 +1879,11 @@
         <v>31</v>
       </c>
       <c r="AL11" s="3"/>
-      <c r="AM11" s="5">
+      <c r="AM11" s="28">
         <v>3</v>
       </c>
-      <c r="AN11" s="6"/>
-      <c r="AO11" s="7"/>
+      <c r="AN11" s="29"/>
+      <c r="AO11" s="30"/>
       <c r="AP11" s="2"/>
     </row>
     <row r="12" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -1926,9 +1926,9 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="8"/>
-      <c r="S12" s="9"/>
-      <c r="T12" s="10"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="33"/>
       <c r="U12" s="4"/>
       <c r="V12" s="3" t="s">
         <v>20</v>
@@ -1969,9 +1969,9 @@
       <c r="AJ12" s="3"/>
       <c r="AK12" s="3"/>
       <c r="AL12" s="3"/>
-      <c r="AM12" s="8"/>
-      <c r="AN12" s="9"/>
-      <c r="AO12" s="10"/>
+      <c r="AM12" s="31"/>
+      <c r="AN12" s="32"/>
+      <c r="AO12" s="33"/>
       <c r="AP12" s="2"/>
     </row>
     <row r="13" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2014,9 +2014,9 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="9"/>
-      <c r="T13" s="10"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="33"/>
       <c r="U13" s="4"/>
       <c r="V13" s="3" t="s">
         <v>21</v>
@@ -2057,9 +2057,9 @@
       <c r="AJ13" s="3"/>
       <c r="AK13" s="3"/>
       <c r="AL13" s="3"/>
-      <c r="AM13" s="8"/>
-      <c r="AN13" s="9"/>
-      <c r="AO13" s="10"/>
+      <c r="AM13" s="31"/>
+      <c r="AN13" s="32"/>
+      <c r="AO13" s="33"/>
       <c r="AP13" s="2"/>
     </row>
     <row r="14" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2104,9 +2104,9 @@
       </c>
       <c r="P14" s="3"/>
       <c r="Q14" s="3"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="12"/>
-      <c r="T14" s="13"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="36"/>
       <c r="U14" s="4"/>
       <c r="V14" s="3" t="s">
         <v>2</v>
@@ -2149,9 +2149,9 @@
       </c>
       <c r="AK14" s="3"/>
       <c r="AL14" s="3"/>
-      <c r="AM14" s="11"/>
-      <c r="AN14" s="12"/>
-      <c r="AO14" s="13"/>
+      <c r="AM14" s="34"/>
+      <c r="AN14" s="35"/>
+      <c r="AO14" s="36"/>
       <c r="AP14" s="2"/>
     </row>
     <row r="15" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -2201,31 +2201,31 @@
     <row r="16" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
-      <c r="C16" s="14">
-        <v>1</v>
-      </c>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14">
-        <v>0</v>
-      </c>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14">
+      <c r="C16" s="27">
+        <v>1</v>
+      </c>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27">
+        <v>0</v>
+      </c>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27">
         <v>5</v>
       </c>
-      <c r="J16" s="14"/>
-      <c r="K16" s="14"/>
-      <c r="L16" s="14">
+      <c r="J16" s="27"/>
+      <c r="K16" s="27"/>
+      <c r="L16" s="27">
         <v>5</v>
       </c>
-      <c r="M16" s="14"/>
-      <c r="N16" s="14"/>
-      <c r="O16" s="14">
+      <c r="M16" s="27"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="27">
         <v>4</v>
       </c>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
+      <c r="P16" s="27"/>
+      <c r="Q16" s="27"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
       <c r="T16" s="3"/>
@@ -2255,21 +2255,21 @@
     <row r="17" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
       <c r="B17" s="3"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
-      <c r="N17" s="14"/>
-      <c r="O17" s="14"/>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+      <c r="O17" s="27"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="27"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
       <c r="T17" s="3"/>
@@ -2299,21 +2299,21 @@
     <row r="18" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
       <c r="B18" s="3"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
-      <c r="K18" s="14"/>
-      <c r="L18" s="14"/>
-      <c r="M18" s="14"/>
-      <c r="N18" s="14"/>
-      <c r="O18" s="14"/>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
+      <c r="C18" s="27"/>
+      <c r="D18" s="27"/>
+      <c r="E18" s="27"/>
+      <c r="F18" s="27"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
+      <c r="J18" s="27"/>
+      <c r="K18" s="27"/>
+      <c r="L18" s="27"/>
+      <c r="M18" s="27"/>
+      <c r="N18" s="27"/>
+      <c r="O18" s="27"/>
+      <c r="P18" s="27"/>
+      <c r="Q18" s="27"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
       <c r="T18" s="3"/>
@@ -2343,21 +2343,21 @@
     <row r="19" spans="1:42" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-      <c r="M19" s="14"/>
-      <c r="N19" s="14"/>
-      <c r="O19" s="14"/>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
+      <c r="M19" s="27"/>
+      <c r="N19" s="27"/>
+      <c r="O19" s="27"/>
+      <c r="P19" s="27"/>
+      <c r="Q19" s="27"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
       <c r="T19" s="3"/>
@@ -2386,16 +2386,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="AM1:AO4"/>
+    <mergeCell ref="AM11:AO14"/>
+    <mergeCell ref="R1:T4"/>
+    <mergeCell ref="R6:T9"/>
+    <mergeCell ref="R11:T14"/>
     <mergeCell ref="C16:E19"/>
     <mergeCell ref="F16:H19"/>
     <mergeCell ref="I16:K19"/>
     <mergeCell ref="L16:N19"/>
     <mergeCell ref="O16:Q19"/>
-    <mergeCell ref="AM1:AO4"/>
-    <mergeCell ref="AM11:AO14"/>
-    <mergeCell ref="R1:T4"/>
-    <mergeCell ref="R6:T9"/>
-    <mergeCell ref="R11:T14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2406,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AO9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2416,596 +2416,596 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="35">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15">
         <v>5</v>
       </c>
-      <c r="G1" s="35">
+      <c r="G1" s="15">
         <v>4</v>
       </c>
-      <c r="H1" s="35">
+      <c r="H1" s="15">
         <v>2</v>
       </c>
-      <c r="I1" s="35" t="s">
+      <c r="I1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="35"/>
-      <c r="K1" s="35" t="s">
+      <c r="J1" s="15"/>
+      <c r="K1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="L1" s="35" t="s">
+      <c r="L1" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="35" t="s">
+      <c r="M1" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="N1" s="35"/>
-      <c r="O1" s="35">
-        <v>1</v>
-      </c>
-      <c r="P1" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q1" s="35">
-        <v>0</v>
-      </c>
-      <c r="R1" s="40" t="s">
+      <c r="N1" s="15"/>
+      <c r="O1" s="15">
+        <v>1</v>
+      </c>
+      <c r="P1" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="15">
+        <v>0</v>
+      </c>
+      <c r="R1" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="T1" s="36" t="s">
+      <c r="T1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="V1" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="W1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="X1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="25"/>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25">
+      <c r="Y1" s="5"/>
+      <c r="Z1" s="5"/>
+      <c r="AA1" s="5">
         <v>5</v>
       </c>
-      <c r="AB1" s="25">
+      <c r="AB1" s="5">
         <v>4</v>
       </c>
-      <c r="AC1" s="25">
+      <c r="AC1" s="5">
         <v>2</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AD1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AE1" s="25"/>
-      <c r="AF1" s="25" t="s">
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AG1" s="25" t="s">
+      <c r="AG1" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="AH1" s="25" t="s">
+      <c r="AH1" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" s="25"/>
-      <c r="AJ1" s="25">
-        <v>1</v>
-      </c>
-      <c r="AK1" s="25">
-        <v>0</v>
-      </c>
-      <c r="AL1" s="25">
-        <v>0</v>
-      </c>
-      <c r="AM1" s="26" t="s">
+      <c r="AI1" s="5"/>
+      <c r="AJ1" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK1" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL1" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="AN1" s="27" t="s">
+      <c r="AN1" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="AO1" s="28" t="s">
+      <c r="AO1" s="8" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="35" t="s">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35">
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15">
         <v>7</v>
       </c>
-      <c r="H2" s="35">
+      <c r="H2" s="15">
         <v>6</v>
       </c>
-      <c r="I2" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35" t="s">
+      <c r="I2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L2" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="35" t="s">
+      <c r="L2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="35"/>
-      <c r="O2" s="35"/>
-      <c r="P2" s="35">
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15">
         <v>5</v>
       </c>
-      <c r="Q2" s="35">
+      <c r="Q2" s="15">
         <v>7</v>
       </c>
-      <c r="R2" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="S2" s="43"/>
-      <c r="T2" s="37"/>
-      <c r="V2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="W2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="X2" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y2" s="25" t="s">
+      <c r="R2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="23"/>
+      <c r="T2" s="17"/>
+      <c r="V2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="Z2" s="25"/>
-      <c r="AA2" s="25"/>
-      <c r="AB2" s="25">
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="5"/>
+      <c r="AB2" s="5">
         <v>7</v>
       </c>
-      <c r="AC2" s="25">
+      <c r="AC2" s="5">
         <v>6</v>
       </c>
-      <c r="AD2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="25"/>
-      <c r="AF2" s="25" t="s">
+      <c r="AD2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="5"/>
+      <c r="AF2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AG2" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="25" t="s">
+      <c r="AG2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AI2" s="25"/>
-      <c r="AJ2" s="25"/>
-      <c r="AK2" s="25">
+      <c r="AI2" s="5"/>
+      <c r="AJ2" s="5"/>
+      <c r="AK2" s="5">
         <v>5</v>
       </c>
-      <c r="AL2" s="25">
+      <c r="AL2" s="5">
         <v>7</v>
       </c>
-      <c r="AM2" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="30"/>
-      <c r="AO2" s="31"/>
+      <c r="AM2" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="10"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="35"/>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15">
         <v>5</v>
       </c>
-      <c r="H3" s="35">
-        <v>1</v>
-      </c>
-      <c r="I3" s="35" t="s">
+      <c r="H3" s="15">
+        <v>1</v>
+      </c>
+      <c r="I3" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35" t="s">
+      <c r="J3" s="15"/>
+      <c r="K3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="M3" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35">
-        <v>1</v>
-      </c>
-      <c r="P3" s="35">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="35">
-        <v>0</v>
-      </c>
-      <c r="R3" s="42" t="s">
+      <c r="L3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="15"/>
+      <c r="O3" s="15">
+        <v>1</v>
+      </c>
+      <c r="P3" s="15">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="15">
+        <v>0</v>
+      </c>
+      <c r="R3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="S3" s="43"/>
-      <c r="T3" s="37"/>
-      <c r="V3" s="25" t="s">
+      <c r="S3" s="23"/>
+      <c r="T3" s="17"/>
+      <c r="V3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="W3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25" t="s">
+      <c r="W3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="X3" s="5"/>
+      <c r="Y3" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="Z3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="25" t="s">
+      <c r="Z3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="AB3" s="25" t="s">
+      <c r="AB3" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="AC3" s="25" t="s">
+      <c r="AC3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AD3" s="25" t="s">
+      <c r="AD3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25" t="s">
+      <c r="AE3" s="5"/>
+      <c r="AF3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AG3" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="AH3" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25">
-        <v>1</v>
-      </c>
-      <c r="AK3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="25">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="29" t="s">
+      <c r="AG3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AH3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="5"/>
+      <c r="AJ3" s="5">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="5">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="AN3" s="30"/>
-      <c r="AO3" s="31"/>
+      <c r="AN3" s="10"/>
+      <c r="AO3" s="11"/>
     </row>
     <row r="4" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" s="35" t="s">
+      <c r="A4" s="15"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35" t="s">
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="L4" s="35" t="s">
+      <c r="L4" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="35" t="s">
+      <c r="M4" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35">
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15">
         <v>2</v>
       </c>
-      <c r="Q4" s="35">
+      <c r="Q4" s="15">
         <v>2</v>
       </c>
-      <c r="R4" s="38" t="s">
+      <c r="R4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="S4" s="44"/>
-      <c r="T4" s="39"/>
-      <c r="V4" s="25"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25" t="s">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="25" t="s">
+      <c r="S4" s="24"/>
+      <c r="T4" s="19"/>
+      <c r="V4" s="5"/>
+      <c r="W4" s="5"/>
+      <c r="X4" s="5"/>
+      <c r="Y4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25" t="s">
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="AG4" s="25" t="s">
+      <c r="AG4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="AH4" s="25" t="s">
+      <c r="AH4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25">
+      <c r="AI4" s="5"/>
+      <c r="AJ4" s="5"/>
+      <c r="AK4" s="5">
         <v>2</v>
       </c>
-      <c r="AL4" s="25">
+      <c r="AL4" s="5">
         <v>2</v>
       </c>
-      <c r="AM4" s="32" t="s">
+      <c r="AM4" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="AN4" s="33"/>
-      <c r="AO4" s="34"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="14"/>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A5" s="45"/>
-      <c r="B5" s="45"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="45"/>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="45"/>
-      <c r="N5" s="45"/>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="45"/>
-      <c r="S5" s="45"/>
-      <c r="T5" s="45"/>
+      <c r="A5" s="25"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25"/>
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
+      <c r="A6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35" t="s">
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="G6" s="35" t="s">
+      <c r="G6" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="H6" s="35" t="s">
+      <c r="H6" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="35"/>
-      <c r="K6" s="35" t="s">
+      <c r="J6" s="15"/>
+      <c r="K6" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="L6" s="35" t="s">
+      <c r="L6" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M6" s="35" t="s">
+      <c r="M6" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="N6" s="35"/>
-      <c r="O6" s="35" t="s">
+      <c r="N6" s="15"/>
+      <c r="O6" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="P6" s="35" t="s">
+      <c r="P6" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="Q6" s="35" t="s">
+      <c r="Q6" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="R6" s="40" t="s">
+      <c r="R6" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="S6" s="41" t="s">
+      <c r="S6" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="T6" s="36" t="s">
+      <c r="T6" s="16" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="35" t="s">
+      <c r="A7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="I7" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="J7" s="35"/>
-      <c r="K7" s="35" t="s">
+      <c r="I7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="L7" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" s="35" t="s">
+      <c r="L7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="M7" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="N7" s="35"/>
-      <c r="O7" s="35"/>
-      <c r="P7" s="35" t="s">
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="Q7" s="35" t="s">
+      <c r="Q7" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="R7" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="S7" s="43"/>
-      <c r="T7" s="37"/>
+      <c r="R7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="S7" s="23"/>
+      <c r="T7" s="17"/>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35" t="s">
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="J8" s="35"/>
-      <c r="K8" s="35" t="s">
+      <c r="J8" s="15"/>
+      <c r="K8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="L8" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="M8" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35" t="s">
+      <c r="L8" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="P8" s="35" t="s">
+      <c r="P8" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="Q8" s="35" t="s">
+      <c r="Q8" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="R8" s="42" t="s">
+      <c r="R8" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="S8" s="43"/>
-      <c r="T8" s="37"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="17"/>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.3">
-      <c r="A9" s="46" t="s">
+      <c r="A9" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="46" t="s">
+      <c r="B9" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="46" t="s">
+      <c r="D9" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="46" t="s">
+      <c r="E9" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="F9" s="46" t="s">
+      <c r="F9" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="G9" s="46" t="s">
+      <c r="G9" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="46" t="s">
+      <c r="H9" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="46" t="s">
+      <c r="I9" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="J9" s="46"/>
-      <c r="K9" s="35" t="s">
+      <c r="J9" s="26"/>
+      <c r="K9" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="L9" s="35" t="s">
+      <c r="L9" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="M9" s="35" t="s">
+      <c r="M9" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35" t="s">
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="Q9" s="35" t="s">
+      <c r="Q9" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="R9" s="38" t="s">
+      <c r="R9" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="S9" s="46"/>
-      <c r="T9" s="46"/>
+      <c r="S9" s="26"/>
+      <c r="T9" s="26"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3018,8 +3018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{159E54EA-16D9-4DA2-844A-BE9A02714367}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView zoomScale="280" zoomScaleNormal="280" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3028,390 +3028,392 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="35" t="s">
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="35" t="s">
+      <c r="D1" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="35"/>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35">
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15">
         <v>4</v>
       </c>
-      <c r="I1" s="35">
+      <c r="I1" s="15">
         <v>5</v>
       </c>
-      <c r="J1" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="K1" s="35"/>
-      <c r="L1" s="35"/>
-      <c r="M1" s="35" t="s">
+      <c r="J1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="35" t="s">
+      <c r="N1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="35" t="s">
+      <c r="O1" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="35"/>
-      <c r="Q1" s="35"/>
-      <c r="R1" s="35">
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15">
         <v>5</v>
       </c>
-      <c r="S1" s="35">
+      <c r="S1" s="15">
         <v>5</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="T1" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="35" t="s">
+      <c r="A2" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="35" t="s">
+      <c r="C2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="35">
+      <c r="F2" s="15"/>
+      <c r="G2" s="15">
         <v>4</v>
       </c>
-      <c r="H2" s="35" t="s">
+      <c r="H2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="35">
+      <c r="I2" s="15">
         <v>2</v>
       </c>
-      <c r="J2" s="35" t="s">
+      <c r="J2" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35" t="s">
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="35" t="s">
+      <c r="N2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="35" t="s">
+      <c r="O2" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="P2" s="35"/>
-      <c r="Q2" s="35">
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15">
         <v>4</v>
       </c>
-      <c r="R2" s="35" t="s">
+      <c r="R2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="35">
+      <c r="S2" s="15">
         <v>3</v>
       </c>
-      <c r="T2" s="35" t="s">
+      <c r="T2" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35" t="s">
+      <c r="A3" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="35">
-        <v>1</v>
-      </c>
-      <c r="E3" s="35"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="35">
-        <v>1</v>
-      </c>
-      <c r="H3" s="35">
-        <v>0</v>
-      </c>
-      <c r="I3" s="35">
-        <v>0</v>
-      </c>
-      <c r="J3" s="35" t="s">
+      <c r="E3" s="15">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15">
+        <v>1</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15">
+        <v>0</v>
+      </c>
+      <c r="J3" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35">
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="15">
         <v>2</v>
       </c>
-      <c r="N3" s="35"/>
-      <c r="O3" s="35"/>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="35">
-        <v>1</v>
-      </c>
-      <c r="R3" s="35">
-        <v>0</v>
-      </c>
-      <c r="S3" s="35">
-        <v>0</v>
-      </c>
-      <c r="T3" s="35" t="s">
+      <c r="N3" s="15"/>
+      <c r="O3" s="15"/>
+      <c r="P3" s="15"/>
+      <c r="Q3" s="15">
+        <v>1</v>
+      </c>
+      <c r="R3" s="15">
+        <v>0</v>
+      </c>
+      <c r="S3" s="15">
+        <v>0</v>
+      </c>
+      <c r="T3" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35">
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15">
         <v>9</v>
       </c>
-      <c r="I4" s="35">
-        <v>0</v>
-      </c>
-      <c r="J4" s="35" t="s">
+      <c r="I4" s="15">
+        <v>0</v>
+      </c>
+      <c r="J4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35" t="s">
+      <c r="K4" s="15"/>
+      <c r="L4" s="15"/>
+      <c r="M4" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
-      <c r="Q4" s="35"/>
-      <c r="R4" s="35">
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15">
         <v>9</v>
       </c>
-      <c r="S4" s="35">
-        <v>0</v>
-      </c>
-      <c r="T4" s="35" t="s">
+      <c r="S4" s="15">
+        <v>0</v>
+      </c>
+      <c r="T4" s="15" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A6" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="35" t="s">
+      <c r="A6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="H6" s="35" t="s">
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="I6" s="35" t="s">
+      <c r="I6" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="J6" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35" t="s">
+      <c r="J6" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="N6" s="35" t="s">
+      <c r="N6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O6" s="35" t="s">
+      <c r="O6" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="P6" s="35"/>
-      <c r="Q6" s="35"/>
-      <c r="R6" s="35" t="s">
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="S6" s="35" t="s">
+      <c r="S6" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="T6" s="35" t="s">
+      <c r="T6" s="15" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A7" s="35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7" s="35" t="s">
+      <c r="A7" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="35" t="s">
+      <c r="C7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="35" t="s">
+      <c r="D7" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E7" s="35" t="s">
+      <c r="E7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35" t="s">
+      <c r="F7" s="15"/>
+      <c r="G7" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="H7" s="35" t="s">
+      <c r="H7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="I7" s="35" t="s">
+      <c r="I7" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="J7" s="35" t="s">
+      <c r="J7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="35"/>
-      <c r="L7" s="35"/>
-      <c r="M7" s="35" t="s">
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="N7" s="35" t="s">
+      <c r="N7" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="O7" s="35" t="s">
+      <c r="O7" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="P7" s="35"/>
-      <c r="Q7" s="35" t="s">
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="R7" s="35" t="s">
+      <c r="R7" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="S7" s="35" t="s">
+      <c r="S7" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="T7" s="35" t="s">
+      <c r="T7" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A8" s="35" t="s">
+      <c r="A8" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="35" t="s">
+      <c r="C8" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="35">
-        <v>1</v>
-      </c>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35" t="s">
+      <c r="D8" s="15">
+        <v>1</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="H8" s="35" t="s">
+      <c r="H8" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="I8" s="35" t="s">
+      <c r="I8" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="J8" s="35" t="s">
+      <c r="J8" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="K8" s="35"/>
-      <c r="L8" s="35"/>
-      <c r="M8" s="35">
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15">
         <v>2</v>
       </c>
-      <c r="N8" s="35"/>
-      <c r="O8" s="35"/>
-      <c r="P8" s="35"/>
-      <c r="Q8" s="35" t="s">
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
+      <c r="P8" s="15"/>
+      <c r="Q8" s="15" t="s">
         <v>92</v>
       </c>
-      <c r="R8" s="35" t="s">
+      <c r="R8" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="S8" s="35" t="s">
+      <c r="S8" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="T8" s="35" t="s">
+      <c r="T8" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A9" s="35" t="s">
+      <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C9" s="35" t="s">
+      <c r="C9" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="H9" s="35" t="s">
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="I9" s="35" t="s">
+      <c r="I9" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="35"/>
-      <c r="L9" s="35"/>
-      <c r="M9" s="35" t="s">
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="N9" s="35"/>
-      <c r="O9" s="35"/>
-      <c r="P9" s="35"/>
-      <c r="Q9" s="35"/>
-      <c r="R9" s="35" t="s">
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="S9" s="35" t="s">
+      <c r="S9" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="T9" s="35" t="s">
+      <c r="T9" s="15" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3424,7 +3426,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF6808A-D3C4-449B-BFA6-52D671B38095}">
   <dimension ref="A1:T9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="K29" sqref="K28:K29"/>
     </sheetView>
   </sheetViews>
@@ -3475,11 +3477,11 @@
         <v>31</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="15">
+      <c r="R1" s="37">
         <v>3</v>
       </c>
-      <c r="S1" s="16"/>
-      <c r="T1" s="17"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="39"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -3521,9 +3523,9 @@
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="18"/>
-      <c r="S2" s="19"/>
-      <c r="T2" s="20"/>
+      <c r="R2" s="40"/>
+      <c r="S2" s="41"/>
+      <c r="T2" s="42"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -3565,9 +3567,9 @@
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
-      <c r="R3" s="18"/>
-      <c r="S3" s="19"/>
-      <c r="T3" s="20"/>
+      <c r="R3" s="40"/>
+      <c r="S3" s="41"/>
+      <c r="T3" s="42"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
@@ -3611,9 +3613,9 @@
       </c>
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
-      <c r="R4" s="21"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="23"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="44"/>
+      <c r="T4" s="45"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
@@ -3842,31 +3844,31 @@
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="24">
-        <v>1</v>
-      </c>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24">
-        <v>0</v>
-      </c>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24">
+      <c r="C1" s="46">
+        <v>1</v>
+      </c>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46">
+        <v>0</v>
+      </c>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46">
         <v>5</v>
       </c>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24">
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46">
         <v>5</v>
       </c>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24"/>
-      <c r="O1" s="24">
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46">
         <v>4</v>
       </c>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -3874,21 +3876,21 @@
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="46"/>
+      <c r="P2" s="46"/>
+      <c r="Q2" s="46"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
@@ -3896,21 +3898,21 @@
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="24"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="24"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
@@ -3918,21 +3920,21 @@
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
+      <c r="C4" s="46"/>
+      <c r="D4" s="46"/>
+      <c r="E4" s="46"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="46"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="46"/>
+      <c r="L4" s="46"/>
+      <c r="M4" s="46"/>
+      <c r="N4" s="46"/>
+      <c r="O4" s="46"/>
+      <c r="P4" s="46"/>
+      <c r="Q4" s="46"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>

</xml_diff>